<commit_message>
sccs primary analysis finished
</commit_message>
<xml_diff>
--- a/3.output/mnd.xlsx
+++ b/3.output/mnd.xlsx
@@ -8,16 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="table 1 demo" sheetId="1" r:id="rId1"/>
+    <sheet name="primary_analysis" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="table_1_demo">'table 1 demo'!$A$1:$J$64</definedName>
+    <definedName name="primary_analysis">'primary_analysis'!$A$1:$K$17</definedName>
   </definedNames>
   <calcPr fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="229">
   <si>
     <t>treatment_column</t>
   </si>
@@ -473,6 +475,237 @@
   </si>
   <si>
     <t>rx_antibiotics=1</t>
+  </si>
+  <si>
+    <t>188</t>
+  </si>
+  <si>
+    <t>1751</t>
+  </si>
+  <si>
+    <t>1.7 (1.3)</t>
+  </si>
+  <si>
+    <t>59.1 (12.3)</t>
+  </si>
+  <si>
+    <t>60.8 (15.3)</t>
+  </si>
+  <si>
+    <t>74 (39.4)</t>
+  </si>
+  <si>
+    <t>608 (34.7)</t>
+  </si>
+  <si>
+    <t>114 (60.6)</t>
+  </si>
+  <si>
+    <t>1143 (65.3)</t>
+  </si>
+  <si>
+    <t>178 (94.7)</t>
+  </si>
+  <si>
+    <t>1417 (80.9)</t>
+  </si>
+  <si>
+    <t>11 (5.9)</t>
+  </si>
+  <si>
+    <t>216 (12.3)</t>
+  </si>
+  <si>
+    <t>46 (2.6)</t>
+  </si>
+  <si>
+    <t>7 (3.7)</t>
+  </si>
+  <si>
+    <t>71 (4.1)</t>
+  </si>
+  <si>
+    <t>16 (8.5)</t>
+  </si>
+  <si>
+    <t>189 (10.8)</t>
+  </si>
+  <si>
+    <t>2 (1.1)</t>
+  </si>
+  <si>
+    <t>104 (5.9)</t>
+  </si>
+  <si>
+    <t>8 (4.3)</t>
+  </si>
+  <si>
+    <t>114 (6.5)</t>
+  </si>
+  <si>
+    <t>5 (2.7)</t>
+  </si>
+  <si>
+    <t>55 (3.1)</t>
+  </si>
+  <si>
+    <t>3 (1.6)</t>
+  </si>
+  <si>
+    <t>12 (6.4)</t>
+  </si>
+  <si>
+    <t>141 (8.1)</t>
+  </si>
+  <si>
+    <t>13 (6.9)</t>
+  </si>
+  <si>
+    <t>219 (12.5)</t>
+  </si>
+  <si>
+    <t>12 (0.7)</t>
+  </si>
+  <si>
+    <t>17 (9)</t>
+  </si>
+  <si>
+    <t>199 (11.4)</t>
+  </si>
+  <si>
+    <t>125 (7.1)</t>
+  </si>
+  <si>
+    <t>153 (8.7)</t>
+  </si>
+  <si>
+    <t>20 (10.6)</t>
+  </si>
+  <si>
+    <t>182 (10.4)</t>
+  </si>
+  <si>
+    <t>40 (21.3)</t>
+  </si>
+  <si>
+    <t>284 (16.2)</t>
+  </si>
+  <si>
+    <t>86 (4.9)</t>
+  </si>
+  <si>
+    <t>4 (2.1)</t>
+  </si>
+  <si>
+    <t>29 (15.4)</t>
+  </si>
+  <si>
+    <t>167 (9.5)</t>
+  </si>
+  <si>
+    <t>18 (9.6)</t>
+  </si>
+  <si>
+    <t>120 (6.9)</t>
+  </si>
+  <si>
+    <t>31 (16.5)</t>
+  </si>
+  <si>
+    <t>262 (15)</t>
+  </si>
+  <si>
+    <t>93 (5.3)</t>
+  </si>
+  <si>
+    <t>53 (3)</t>
+  </si>
+  <si>
+    <t>32 (17)</t>
+  </si>
+  <si>
+    <t>434 (24.8)</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>MeanEstimate</t>
+  </si>
+  <si>
+    <t>MeanLowerCL</t>
+  </si>
+  <si>
+    <t>MeanUpperCL</t>
+  </si>
+  <si>
+    <t>LBetaEstimate</t>
+  </si>
+  <si>
+    <t>StdErr</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>LBetaLowerCL</t>
+  </si>
+  <si>
+    <t>LBetaUpperCL</t>
+  </si>
+  <si>
+    <t>ChiSq</t>
+  </si>
+  <si>
+    <t>ProbChiSq</t>
+  </si>
+  <si>
+    <t>strx_30b</t>
+  </si>
+  <si>
+    <t>Exp(strx_30b)</t>
+  </si>
+  <si>
+    <t>strx_0a</t>
+  </si>
+  <si>
+    <t>Exp(strx_0a)</t>
+  </si>
+  <si>
+    <t>strx_30a</t>
+  </si>
+  <si>
+    <t>Exp(strx_30a)</t>
+  </si>
+  <si>
+    <t>strx_60a</t>
+  </si>
+  <si>
+    <t>Exp(strx_60a)</t>
+  </si>
+  <si>
+    <t>strx_90a</t>
+  </si>
+  <si>
+    <t>Exp(strx_90a)</t>
+  </si>
+  <si>
+    <t>strx_120a</t>
+  </si>
+  <si>
+    <t>Exp(strx_120a)</t>
+  </si>
+  <si>
+    <t>strx_150a</t>
+  </si>
+  <si>
+    <t>Exp(strx_150a)</t>
+  </si>
+  <si>
+    <t>strx_180a</t>
+  </si>
+  <si>
+    <t>Exp(strx_180a)</t>
   </si>
 </sst>
 </file>
@@ -856,10 +1089,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>152</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>153</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -870,22 +1103,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3">
-        <v>2.174063400576369</v>
+        <v>2.1741861793260995</v>
       </c>
       <c r="D3">
-        <v>1.69425259079693</v>
+        <v>1.6885959028233297</v>
       </c>
       <c r="E3">
-        <v>1.7696078431372548</v>
+        <v>1.7340425531914894</v>
       </c>
       <c r="F3">
-        <v>1.2830297590846453</v>
+        <v>1.3054843747532932</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
@@ -894,7 +1127,7 @@
         <v>-.4</v>
       </c>
       <c r="I3">
-        <v>-26.9</v>
+        <v>-29.2</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
@@ -902,31 +1135,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>155</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>156</v>
       </c>
       <c r="C4">
-        <v>60.7343042052047</v>
+        <v>60.765048700048595</v>
       </c>
       <c r="D4">
-        <v>15.349720369018703</v>
+        <v>15.301047409767273</v>
       </c>
       <c r="E4">
-        <v>59.490934224476966</v>
+        <v>59.09876651084221</v>
       </c>
       <c r="F4">
-        <v>12.041544438721125</v>
+        <v>12.255418781253594</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
       </c>
       <c r="H4">
-        <v>-1.2</v>
+        <v>-1.7</v>
       </c>
       <c r="I4">
-        <v>-9</v>
+        <v>-12</v>
       </c>
       <c r="J4" t="s">
         <v>20</v>
@@ -934,31 +1167,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>157</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>158</v>
       </c>
       <c r="C5">
-        <v>601</v>
+        <v>608</v>
       </c>
       <c r="D5">
-        <v>34.63976945244957</v>
+        <v>34.72301541976014</v>
       </c>
       <c r="E5">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F5">
-        <v>39.705882352941174</v>
+        <v>39.361702127659576</v>
       </c>
       <c r="G5" t="s">
         <v>23</v>
       </c>
       <c r="H5">
-        <v>5.1</v>
+        <v>4.6</v>
       </c>
       <c r="I5">
-        <v>10.5</v>
+        <v>9.6</v>
       </c>
       <c r="J5" t="s">
         <v>24</v>
@@ -966,31 +1199,31 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>160</v>
       </c>
       <c r="C6">
-        <v>1134</v>
+        <v>1143</v>
       </c>
       <c r="D6">
-        <v>65.36023054755043</v>
+        <v>65.27698458023987</v>
       </c>
       <c r="E6">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F6">
-        <v>60.294117647058826</v>
+        <v>60.638297872340424</v>
       </c>
       <c r="G6" t="s">
         <v>23</v>
       </c>
       <c r="H6">
-        <v>-5.1</v>
+        <v>-4.6</v>
       </c>
       <c r="I6">
-        <v>-10.5</v>
+        <v>-9.6</v>
       </c>
       <c r="J6" t="s">
         <v>27</v>
@@ -998,31 +1231,31 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>162</v>
       </c>
       <c r="C7">
-        <v>1400</v>
+        <v>1417</v>
       </c>
       <c r="D7">
-        <v>80.69164265129683</v>
+        <v>80.92518560822387</v>
       </c>
       <c r="E7">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="F7">
-        <v>95.58823529411765</v>
+        <v>94.68085106382979</v>
       </c>
       <c r="G7" t="s">
         <v>23</v>
       </c>
       <c r="H7">
-        <v>14.9</v>
+        <v>13.8</v>
       </c>
       <c r="I7">
-        <v>47.3</v>
+        <v>43</v>
       </c>
       <c r="J7" t="s">
         <v>30</v>
@@ -1039,22 +1272,22 @@
         <v>73</v>
       </c>
       <c r="D8">
-        <v>4.207492795389049</v>
+        <v>4.169046259280411</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>.49019607843137253</v>
+        <v>.5319148936170213</v>
       </c>
       <c r="G8" t="s">
         <v>23</v>
       </c>
       <c r="H8">
-        <v>-3.7</v>
+        <v>-3.6</v>
       </c>
       <c r="I8">
-        <v>-24.7</v>
+        <v>-24.2</v>
       </c>
       <c r="J8" t="s">
         <v>33</v>
@@ -1062,31 +1295,31 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>164</v>
       </c>
       <c r="C9">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D9">
-        <v>12.507204610951009</v>
+        <v>12.335808109651628</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F9">
-        <v>4.901960784313726</v>
+        <v>5.851063829787234</v>
       </c>
       <c r="G9" t="s">
         <v>23</v>
       </c>
       <c r="H9">
-        <v>-7.6</v>
+        <v>-6.5</v>
       </c>
       <c r="I9">
-        <v>-27.2</v>
+        <v>-22.7</v>
       </c>
       <c r="J9" t="s">
         <v>36</v>
@@ -1103,7 +1336,7 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>.5187319884726225</v>
+        <v>.5139920045688178</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1129,28 +1362,28 @@
         <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>165</v>
       </c>
       <c r="C11">
         <v>46</v>
       </c>
       <c r="D11">
-        <v>2.6512968299711814</v>
+        <v>2.627070245573958</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11">
-        <v>.49019607843137253</v>
+        <v>.5319148936170213</v>
       </c>
       <c r="G11" t="s">
         <v>23</v>
       </c>
       <c r="H11">
-        <v>-2.2</v>
+        <v>-2.1</v>
       </c>
       <c r="I11">
-        <v>-17.4</v>
+        <v>-16.9</v>
       </c>
       <c r="J11" t="s">
         <v>41</v>
@@ -1167,13 +1400,13 @@
         <v>40</v>
       </c>
       <c r="D12">
-        <v>2.3054755043227666</v>
+        <v>2.2844089091947457</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12">
-        <v>.49019607843137253</v>
+        <v>.5319148936170213</v>
       </c>
       <c r="G12" t="s">
         <v>23</v>
@@ -1182,7 +1415,7 @@
         <v>-1.8</v>
       </c>
       <c r="I12">
-        <v>-15.5</v>
+        <v>-14.9</v>
       </c>
       <c r="J12" t="s">
         <v>43</v>
@@ -1199,7 +1432,7 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>.05763688760806916</v>
+        <v>.05711022272986865</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1231,22 +1464,22 @@
         <v>10</v>
       </c>
       <c r="D14">
-        <v>.5763688760806917</v>
+        <v>.5711022272986864</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14">
-        <v>.49019607843137253</v>
+        <v>.5319148936170213</v>
       </c>
       <c r="G14" t="s">
         <v>23</v>
       </c>
       <c r="H14">
-        <v>-.1</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>-1.2</v>
+        <v>-.5</v>
       </c>
       <c r="J14" t="s">
         <v>47</v>
@@ -1254,31 +1487,31 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>166</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>167</v>
       </c>
       <c r="C15">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D15">
-        <v>4.034582132564841</v>
+        <v>4.054825813820674</v>
       </c>
       <c r="E15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15">
-        <v>3.9215686274509802</v>
+        <v>3.723404255319149</v>
       </c>
       <c r="G15" t="s">
         <v>23</v>
       </c>
       <c r="H15">
-        <v>-.1</v>
+        <v>-.3</v>
       </c>
       <c r="I15">
-        <v>-.6</v>
+        <v>-1.7</v>
       </c>
       <c r="J15" t="s">
         <v>50</v>
@@ -1295,7 +1528,7 @@
         <v>26</v>
       </c>
       <c r="D16">
-        <v>1.4985590778097984</v>
+        <v>1.4848657909765848</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1327,7 +1560,7 @@
         <v>9</v>
       </c>
       <c r="D17">
-        <v>.5187319884726225</v>
+        <v>.5139920045688178</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1350,31 +1583,31 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>168</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>169</v>
       </c>
       <c r="C18">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D18">
-        <v>10.778097982708934</v>
+        <v>10.793832095945174</v>
       </c>
       <c r="E18">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F18">
-        <v>8.823529411764707</v>
+        <v>8.51063829787234</v>
       </c>
       <c r="G18" t="s">
         <v>23</v>
       </c>
       <c r="H18">
-        <v>-2</v>
+        <v>-2.3</v>
       </c>
       <c r="I18">
-        <v>-6.6</v>
+        <v>-7.7</v>
       </c>
       <c r="J18" t="s">
         <v>56</v>
@@ -1382,31 +1615,31 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>170</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>171</v>
       </c>
       <c r="C19">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D19">
-        <v>5.936599423631124</v>
+        <v>5.939463163906339</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19">
-        <v>1.4705882352941178</v>
+        <v>1.0638297872340425</v>
       </c>
       <c r="G19" t="s">
         <v>23</v>
       </c>
       <c r="H19">
-        <v>-4.5</v>
+        <v>-4.9</v>
       </c>
       <c r="I19">
-        <v>-23.8</v>
+        <v>-26.8</v>
       </c>
       <c r="J19" t="s">
         <v>59</v>
@@ -1423,7 +1656,7 @@
         <v>11</v>
       </c>
       <c r="D20">
-        <v>.6340057636887608</v>
+        <v>.6282124500285551</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1438,7 +1671,7 @@
         <v>-.6</v>
       </c>
       <c r="I20">
-        <v>-11.3</v>
+        <v>-11.2</v>
       </c>
       <c r="J20" t="s">
         <v>61</v>
@@ -1446,7 +1679,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>170</v>
       </c>
       <c r="B21" t="s">
         <v>63</v>
@@ -1455,22 +1688,22 @@
         <v>42</v>
       </c>
       <c r="D21">
-        <v>2.4207492795389047</v>
+        <v>2.3986293546544832</v>
       </c>
       <c r="E21">
         <v>2</v>
       </c>
       <c r="F21">
-        <v>.9803921568627451</v>
+        <v>1.0638297872340425</v>
       </c>
       <c r="G21" t="s">
         <v>23</v>
       </c>
       <c r="H21">
-        <v>-1.4</v>
+        <v>-1.3</v>
       </c>
       <c r="I21">
-        <v>-11.2</v>
+        <v>-10.2</v>
       </c>
       <c r="J21" t="s">
         <v>64</v>
@@ -1478,31 +1711,31 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>172</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>173</v>
       </c>
       <c r="C22">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D22">
-        <v>6.512968299711815</v>
+        <v>6.510565391205025</v>
       </c>
       <c r="E22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22">
-        <v>4.411764705882353</v>
+        <v>4.25531914893617</v>
       </c>
       <c r="G22" t="s">
         <v>23</v>
       </c>
       <c r="H22">
-        <v>-2.1</v>
+        <v>-2.3</v>
       </c>
       <c r="I22">
-        <v>-9.3</v>
+        <v>-10</v>
       </c>
       <c r="J22" t="s">
         <v>67</v>
@@ -1519,7 +1752,7 @@
         <v>19</v>
       </c>
       <c r="D23">
-        <v>1.095100864553314</v>
+        <v>1.0850942318675043</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1534,7 +1767,7 @@
         <v>-1.1</v>
       </c>
       <c r="I23">
-        <v>-14.9</v>
+        <v>-14.8</v>
       </c>
       <c r="J23" t="s">
         <v>69</v>
@@ -1551,7 +1784,7 @@
         <v>8</v>
       </c>
       <c r="D24">
-        <v>.4610951008645533</v>
+        <v>.4568817818389492</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1583,7 +1816,7 @@
         <v>3</v>
       </c>
       <c r="D25">
-        <v>.1729106628242075</v>
+        <v>.17133066818960593</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1615,7 +1848,7 @@
         <v>2</v>
       </c>
       <c r="D26">
-        <v>.11527377521613832</v>
+        <v>.1142204454597373</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1638,31 +1871,31 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>174</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>175</v>
       </c>
       <c r="C27">
         <v>55</v>
       </c>
       <c r="D27">
-        <v>3.170028818443804</v>
+        <v>3.1410622501427756</v>
       </c>
       <c r="E27">
         <v>5</v>
       </c>
       <c r="F27">
-        <v>2.450980392156863</v>
+        <v>2.6595744680851063</v>
       </c>
       <c r="G27" t="s">
         <v>23</v>
       </c>
       <c r="H27">
-        <v>-.7</v>
+        <v>-.5</v>
       </c>
       <c r="I27">
-        <v>-4.4</v>
+        <v>-2.9</v>
       </c>
       <c r="J27" t="s">
         <v>78</v>
@@ -1679,7 +1912,7 @@
         <v>7</v>
       </c>
       <c r="D28">
-        <v>.4034582132564842</v>
+        <v>.3997715591090805</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1702,7 +1935,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>176</v>
       </c>
       <c r="B29" t="s">
         <v>81</v>
@@ -1711,22 +1944,22 @@
         <v>78</v>
       </c>
       <c r="D29">
-        <v>4.495677233429395</v>
+        <v>4.454597372929754</v>
       </c>
       <c r="E29">
         <v>3</v>
       </c>
       <c r="F29">
-        <v>1.4705882352941178</v>
+        <v>1.5957446808510638</v>
       </c>
       <c r="G29" t="s">
         <v>23</v>
       </c>
       <c r="H29">
-        <v>-3</v>
+        <v>-2.9</v>
       </c>
       <c r="I29">
-        <v>-17.9</v>
+        <v>-16.7</v>
       </c>
       <c r="J29" t="s">
         <v>82</v>
@@ -1743,7 +1976,7 @@
         <v>2</v>
       </c>
       <c r="D30">
-        <v>.11527377521613832</v>
+        <v>.1142204454597373</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1766,31 +1999,31 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>177</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>178</v>
       </c>
       <c r="C31">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D31">
-        <v>8.011527377521613</v>
+        <v>8.052541404911478</v>
       </c>
       <c r="E31">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F31">
-        <v>6.862745098039215</v>
+        <v>6.382978723404255</v>
       </c>
       <c r="G31" t="s">
         <v>23</v>
       </c>
       <c r="H31">
-        <v>-1.1</v>
+        <v>-1.7</v>
       </c>
       <c r="I31">
-        <v>-4.4</v>
+        <v>-6.5</v>
       </c>
       <c r="J31" t="s">
         <v>86</v>
@@ -1807,7 +2040,7 @@
         <v>32</v>
       </c>
       <c r="D32">
-        <v>1.8443804034582132</v>
+        <v>1.8275271273557967</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1822,7 +2055,7 @@
         <v>-1.8</v>
       </c>
       <c r="I32">
-        <v>-19.4</v>
+        <v>-19.3</v>
       </c>
       <c r="J32" t="s">
         <v>88</v>
@@ -1830,7 +2063,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>176</v>
       </c>
       <c r="B33" t="s">
         <v>81</v>
@@ -1839,22 +2072,22 @@
         <v>78</v>
       </c>
       <c r="D33">
-        <v>4.495677233429395</v>
+        <v>4.454597372929754</v>
       </c>
       <c r="E33">
         <v>3</v>
       </c>
       <c r="F33">
-        <v>1.4705882352941178</v>
+        <v>1.5957446808510638</v>
       </c>
       <c r="G33" t="s">
         <v>23</v>
       </c>
       <c r="H33">
-        <v>-3</v>
+        <v>-2.9</v>
       </c>
       <c r="I33">
-        <v>-17.9</v>
+        <v>-16.7</v>
       </c>
       <c r="J33" t="s">
         <v>89</v>
@@ -1862,31 +2095,31 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>179</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="C34">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D34">
-        <v>12.564841498559078</v>
+        <v>12.507138777841234</v>
       </c>
       <c r="E34">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F34">
-        <v>6.862745098039215</v>
+        <v>6.914893617021277</v>
       </c>
       <c r="G34" t="s">
         <v>23</v>
       </c>
       <c r="H34">
-        <v>-5.7</v>
+        <v>-5.6</v>
       </c>
       <c r="I34">
-        <v>-19.3</v>
+        <v>-19</v>
       </c>
       <c r="J34" t="s">
         <v>91</v>
@@ -1894,31 +2127,31 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>181</v>
       </c>
       <c r="C35">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D35">
-        <v>.6340057636887608</v>
+        <v>.6853226727584237</v>
       </c>
       <c r="E35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35">
-        <v>.9803921568627451</v>
+        <v>.5319148936170213</v>
       </c>
       <c r="G35" t="s">
         <v>23</v>
       </c>
       <c r="H35">
-        <v>.3</v>
+        <v>-.2</v>
       </c>
       <c r="I35">
-        <v>3.9</v>
+        <v>-2</v>
       </c>
       <c r="J35" t="s">
         <v>92</v>
@@ -1935,7 +2168,7 @@
         <v>1</v>
       </c>
       <c r="D36">
-        <v>.05763688760806916</v>
+        <v>.05711022272986865</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1958,7 +2191,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>62</v>
+        <v>170</v>
       </c>
       <c r="B37" t="s">
         <v>72</v>
@@ -1967,22 +2200,22 @@
         <v>3</v>
       </c>
       <c r="D37">
-        <v>.1729106628242075</v>
+        <v>.17133066818960593</v>
       </c>
       <c r="E37">
         <v>2</v>
       </c>
       <c r="F37">
-        <v>.9803921568627451</v>
+        <v>1.0638297872340425</v>
       </c>
       <c r="G37" t="s">
         <v>23</v>
       </c>
       <c r="H37">
-        <v>.8</v>
+        <v>.9</v>
       </c>
       <c r="I37">
-        <v>10.7</v>
+        <v>11.4</v>
       </c>
       <c r="J37" t="s">
         <v>94</v>
@@ -1990,7 +2223,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>170</v>
       </c>
       <c r="B38" t="s">
         <v>95</v>
@@ -1999,22 +2232,22 @@
         <v>33</v>
       </c>
       <c r="D38">
-        <v>1.9020172910662825</v>
+        <v>1.8846373500856652</v>
       </c>
       <c r="E38">
         <v>2</v>
       </c>
       <c r="F38">
-        <v>.9803921568627451</v>
+        <v>1.0638297872340425</v>
       </c>
       <c r="G38" t="s">
         <v>23</v>
       </c>
       <c r="H38">
-        <v>-.9</v>
+        <v>-.8</v>
       </c>
       <c r="I38">
-        <v>-7.7</v>
+        <v>-6.8</v>
       </c>
       <c r="J38" t="s">
         <v>96</v>
@@ -2022,31 +2255,31 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>182</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>183</v>
       </c>
       <c r="C39">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D39">
-        <v>11.354466858789625</v>
+        <v>11.36493432324386</v>
       </c>
       <c r="E39">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F39">
-        <v>9.313725490196079</v>
+        <v>9.042553191489361</v>
       </c>
       <c r="G39" t="s">
         <v>23</v>
       </c>
       <c r="H39">
-        <v>-2</v>
+        <v>-2.3</v>
       </c>
       <c r="I39">
-        <v>-6.7</v>
+        <v>-7.7</v>
       </c>
       <c r="J39" t="s">
         <v>99</v>
@@ -2054,31 +2287,31 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>65</v>
+        <v>172</v>
       </c>
       <c r="B40" t="s">
-        <v>100</v>
+        <v>184</v>
       </c>
       <c r="C40">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D40">
-        <v>7.1469740634005765</v>
+        <v>7.138777841233581</v>
       </c>
       <c r="E40">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F40">
-        <v>4.411764705882353</v>
+        <v>4.25531914893617</v>
       </c>
       <c r="G40" t="s">
         <v>23</v>
       </c>
       <c r="H40">
-        <v>-2.7</v>
+        <v>-2.9</v>
       </c>
       <c r="I40">
-        <v>-11.7</v>
+        <v>-12.5</v>
       </c>
       <c r="J40" t="s">
         <v>101</v>
@@ -2086,31 +2319,31 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>177</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>178</v>
       </c>
       <c r="C41">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D41">
-        <v>8.011527377521613</v>
+        <v>8.052541404911478</v>
       </c>
       <c r="E41">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F41">
-        <v>6.862745098039215</v>
+        <v>6.382978723404255</v>
       </c>
       <c r="G41" t="s">
         <v>23</v>
       </c>
       <c r="H41">
-        <v>-1.1</v>
+        <v>-1.7</v>
       </c>
       <c r="I41">
-        <v>-4.4</v>
+        <v>-6.5</v>
       </c>
       <c r="J41" t="s">
         <v>102</v>
@@ -2118,31 +2351,31 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>97</v>
+        <v>182</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>185</v>
       </c>
       <c r="C42">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D42">
-        <v>8.703170028818445</v>
+        <v>8.737864077669903</v>
       </c>
       <c r="E42">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F42">
-        <v>9.313725490196079</v>
+        <v>9.042553191489361</v>
       </c>
       <c r="G42" t="s">
         <v>23</v>
       </c>
       <c r="H42">
-        <v>.6</v>
+        <v>.3</v>
       </c>
       <c r="I42">
-        <v>2.1</v>
+        <v>1.1</v>
       </c>
       <c r="J42" t="s">
         <v>104</v>
@@ -2150,31 +2383,31 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>186</v>
       </c>
       <c r="B43" t="s">
-        <v>106</v>
+        <v>187</v>
       </c>
       <c r="C43">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D43">
-        <v>10.37463976945245</v>
+        <v>10.394060536836093</v>
       </c>
       <c r="E43">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F43">
-        <v>10.784313725490197</v>
+        <v>10.638297872340425</v>
       </c>
       <c r="G43" t="s">
         <v>23</v>
       </c>
       <c r="H43">
-        <v>.4</v>
+        <v>.2</v>
       </c>
       <c r="I43">
-        <v>1.3</v>
+        <v>.8</v>
       </c>
       <c r="J43" t="s">
         <v>107</v>
@@ -2182,31 +2415,31 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>108</v>
+        <v>188</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>189</v>
       </c>
       <c r="C44">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D44">
-        <v>16.311239193083573</v>
+        <v>16.219303255282696</v>
       </c>
       <c r="E44">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F44">
-        <v>20.098039215686274</v>
+        <v>21.27659574468085</v>
       </c>
       <c r="G44" t="s">
         <v>23</v>
       </c>
       <c r="H44">
-        <v>3.8</v>
+        <v>5.1</v>
       </c>
       <c r="I44">
-        <v>9.8</v>
+        <v>13</v>
       </c>
       <c r="J44" t="s">
         <v>110</v>
@@ -2214,31 +2447,31 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>174</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>190</v>
       </c>
       <c r="C45">
         <v>86</v>
       </c>
       <c r="D45">
-        <v>4.956772334293948</v>
+        <v>4.911479154768704</v>
       </c>
       <c r="E45">
         <v>5</v>
       </c>
       <c r="F45">
-        <v>2.450980392156863</v>
+        <v>2.6595744680851063</v>
       </c>
       <c r="G45" t="s">
         <v>23</v>
       </c>
       <c r="H45">
-        <v>-2.5</v>
+        <v>-2.3</v>
       </c>
       <c r="I45">
-        <v>-13.3</v>
+        <v>-11.8</v>
       </c>
       <c r="J45" t="s">
         <v>112</v>
@@ -2246,7 +2479,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>191</v>
       </c>
       <c r="B46" t="s">
         <v>114</v>
@@ -2255,22 +2488,22 @@
         <v>72</v>
       </c>
       <c r="D46">
-        <v>4.14985590778098</v>
+        <v>4.111936036550542</v>
       </c>
       <c r="E46">
         <v>4</v>
       </c>
       <c r="F46">
-        <v>1.9607843137254901</v>
+        <v>2.127659574468085</v>
       </c>
       <c r="G46" t="s">
         <v>23</v>
       </c>
       <c r="H46">
-        <v>-2.2</v>
+        <v>-2</v>
       </c>
       <c r="I46">
-        <v>-12.7</v>
+        <v>-11.4</v>
       </c>
       <c r="J46" t="s">
         <v>115</v>
@@ -2278,31 +2511,31 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>116</v>
+        <v>192</v>
       </c>
       <c r="B47" t="s">
-        <v>117</v>
+        <v>193</v>
       </c>
       <c r="C47">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D47">
-        <v>9.452449567723344</v>
+        <v>9.537407195888065</v>
       </c>
       <c r="E47">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F47">
-        <v>15.686274509803921</v>
+        <v>15.425531914893616</v>
       </c>
       <c r="G47" t="s">
         <v>23</v>
       </c>
       <c r="H47">
-        <v>6.2</v>
+        <v>5.9</v>
       </c>
       <c r="I47">
-        <v>18.9</v>
+        <v>17.9</v>
       </c>
       <c r="J47" t="s">
         <v>118</v>
@@ -2319,7 +2552,7 @@
         <v>32</v>
       </c>
       <c r="D48">
-        <v>1.8443804034582132</v>
+        <v>1.8275271273557967</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -2334,7 +2567,7 @@
         <v>-1.8</v>
       </c>
       <c r="I48">
-        <v>-19.4</v>
+        <v>-19.3</v>
       </c>
       <c r="J48" t="s">
         <v>119</v>
@@ -2342,31 +2575,31 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>194</v>
+      </c>
+      <c r="B49" t="s">
+        <v>195</v>
+      </c>
+      <c r="C49">
         <v>120</v>
       </c>
-      <c r="B49" t="s">
-        <v>121</v>
-      </c>
-      <c r="C49">
-        <v>118</v>
-      </c>
       <c r="D49">
-        <v>6.801152737752162</v>
+        <v>6.853226727584238</v>
       </c>
       <c r="E49">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F49">
-        <v>9.803921568627452</v>
+        <v>9.574468085106384</v>
       </c>
       <c r="G49" t="s">
         <v>23</v>
       </c>
       <c r="H49">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="I49">
-        <v>10.9</v>
+        <v>9.9</v>
       </c>
       <c r="J49" t="s">
         <v>122</v>
@@ -2383,7 +2616,7 @@
         <v>13</v>
       </c>
       <c r="D50">
-        <v>.7492795389048992</v>
+        <v>.7424328954882924</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -2398,7 +2631,7 @@
         <v>-.7</v>
       </c>
       <c r="I50">
-        <v>-12.3</v>
+        <v>-12.2</v>
       </c>
       <c r="J50" t="s">
         <v>124</v>
@@ -2415,7 +2648,7 @@
         <v>14</v>
       </c>
       <c r="D51">
-        <v>.8069164265129684</v>
+        <v>.799543118218161</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -2430,7 +2663,7 @@
         <v>-.8</v>
       </c>
       <c r="I51">
-        <v>-12.8</v>
+        <v>-12.7</v>
       </c>
       <c r="J51" t="s">
         <v>126</v>
@@ -2447,13 +2680,13 @@
         <v>21</v>
       </c>
       <c r="D52">
-        <v>1.2103746397694524</v>
+        <v>1.1993146773272416</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
       <c r="F52">
-        <v>.49019607843137253</v>
+        <v>.5319148936170213</v>
       </c>
       <c r="G52" t="s">
         <v>23</v>
@@ -2462,7 +2695,7 @@
         <v>-.7</v>
       </c>
       <c r="I52">
-        <v>-7.8</v>
+        <v>-7.2</v>
       </c>
       <c r="J52" t="s">
         <v>128</v>
@@ -2479,7 +2712,7 @@
         <v>36</v>
       </c>
       <c r="D53">
-        <v>2.07492795389049</v>
+        <v>2.055968018275271</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -2494,7 +2727,7 @@
         <v>-2.1</v>
       </c>
       <c r="I53">
-        <v>-20.6</v>
+        <v>-20.5</v>
       </c>
       <c r="J53" t="s">
         <v>130</v>
@@ -2502,31 +2735,31 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>131</v>
+        <v>196</v>
       </c>
       <c r="B54" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
       <c r="C54">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D54">
-        <v>14.927953890489913</v>
+        <v>14.962878355225586</v>
       </c>
       <c r="E54">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F54">
-        <v>16.666666666666668</v>
+        <v>16.48936170212766</v>
       </c>
       <c r="G54" t="s">
         <v>23</v>
       </c>
       <c r="H54">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="I54">
-        <v>4.8</v>
+        <v>4.2</v>
       </c>
       <c r="J54" t="s">
         <v>133</v>
@@ -2543,7 +2776,7 @@
         <v>26</v>
       </c>
       <c r="D55">
-        <v>1.4985590778097984</v>
+        <v>1.4848657909765848</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -2566,31 +2799,31 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B56" t="s">
-        <v>60</v>
+        <v>181</v>
       </c>
       <c r="C56">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D56">
-        <v>.6340057636887608</v>
+        <v>.6853226727584237</v>
       </c>
       <c r="E56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56">
-        <v>.9803921568627451</v>
+        <v>.5319148936170213</v>
       </c>
       <c r="G56" t="s">
         <v>23</v>
       </c>
       <c r="H56">
-        <v>.3</v>
+        <v>-.2</v>
       </c>
       <c r="I56">
-        <v>3.9</v>
+        <v>-2</v>
       </c>
       <c r="J56" t="s">
         <v>135</v>
@@ -2598,7 +2831,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>174</v>
       </c>
       <c r="B57" t="s">
         <v>136</v>
@@ -2607,22 +2840,22 @@
         <v>80</v>
       </c>
       <c r="D57">
-        <v>4.610951008645533</v>
+        <v>4.568817818389491</v>
       </c>
       <c r="E57">
         <v>5</v>
       </c>
       <c r="F57">
-        <v>2.450980392156863</v>
+        <v>2.6595744680851063</v>
       </c>
       <c r="G57" t="s">
         <v>23</v>
       </c>
       <c r="H57">
-        <v>-2.2</v>
+        <v>-1.9</v>
       </c>
       <c r="I57">
-        <v>-11.7</v>
+        <v>-10.2</v>
       </c>
       <c r="J57" t="s">
         <v>137</v>
@@ -2630,7 +2863,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
       <c r="B58" t="s">
         <v>100</v>
@@ -2639,22 +2872,22 @@
         <v>124</v>
       </c>
       <c r="D58">
-        <v>7.1469740634005765</v>
+        <v>7.081667618503712</v>
       </c>
       <c r="E58">
         <v>12</v>
       </c>
       <c r="F58">
-        <v>5.882352941176471</v>
+        <v>6.382978723404255</v>
       </c>
       <c r="G58" t="s">
         <v>23</v>
       </c>
       <c r="H58">
-        <v>-1.3</v>
+        <v>-.7</v>
       </c>
       <c r="I58">
-        <v>-5.1</v>
+        <v>-2.8</v>
       </c>
       <c r="J58" t="s">
         <v>139</v>
@@ -2671,22 +2904,22 @@
         <v>17</v>
       </c>
       <c r="D59">
-        <v>.9798270893371758</v>
+        <v>.970873786407767</v>
       </c>
       <c r="E59">
         <v>1</v>
       </c>
       <c r="F59">
-        <v>.49019607843137253</v>
+        <v>.5319148936170213</v>
       </c>
       <c r="G59" t="s">
         <v>23</v>
       </c>
       <c r="H59">
-        <v>-.5</v>
+        <v>-.4</v>
       </c>
       <c r="I59">
-        <v>-5.7</v>
+        <v>-5.1</v>
       </c>
       <c r="J59" t="s">
         <v>141</v>
@@ -2694,31 +2927,31 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>54</v>
+        <v>194</v>
       </c>
       <c r="B60" t="s">
-        <v>142</v>
+        <v>198</v>
       </c>
       <c r="C60">
         <v>93</v>
       </c>
       <c r="D60">
-        <v>5.360230547550432</v>
+        <v>5.311250713877784</v>
       </c>
       <c r="E60">
         <v>18</v>
       </c>
       <c r="F60">
-        <v>8.823529411764707</v>
+        <v>9.574468085106384</v>
       </c>
       <c r="G60" t="s">
         <v>23</v>
       </c>
       <c r="H60">
-        <v>3.5</v>
+        <v>4.3</v>
       </c>
       <c r="I60">
-        <v>13.5</v>
+        <v>16.3</v>
       </c>
       <c r="J60" t="s">
         <v>143</v>
@@ -2726,7 +2959,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>176</v>
       </c>
       <c r="B61" t="s">
         <v>63</v>
@@ -2735,22 +2968,22 @@
         <v>42</v>
       </c>
       <c r="D61">
-        <v>2.4207492795389047</v>
+        <v>2.3986293546544832</v>
       </c>
       <c r="E61">
         <v>3</v>
       </c>
       <c r="F61">
-        <v>1.4705882352941178</v>
+        <v>1.5957446808510638</v>
       </c>
       <c r="G61" t="s">
         <v>23</v>
       </c>
       <c r="H61">
-        <v>-1</v>
+        <v>-.8</v>
       </c>
       <c r="I61">
-        <v>-6.9</v>
+        <v>-5.7</v>
       </c>
       <c r="J61" t="s">
         <v>144</v>
@@ -2758,31 +2991,31 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="B62" t="s">
-        <v>146</v>
+        <v>199</v>
       </c>
       <c r="C62">
         <v>53</v>
       </c>
       <c r="D62">
-        <v>3.0547550432276656</v>
+        <v>3.026841804683038</v>
       </c>
       <c r="E62">
         <v>7</v>
       </c>
       <c r="F62">
-        <v>3.4313725490196076</v>
+        <v>3.723404255319149</v>
       </c>
       <c r="G62" t="s">
         <v>23</v>
       </c>
       <c r="H62">
-        <v>.4</v>
+        <v>.7</v>
       </c>
       <c r="I62">
-        <v>2.1</v>
+        <v>3.9</v>
       </c>
       <c r="J62" t="s">
         <v>147</v>
@@ -2799,13 +3032,13 @@
         <v>33</v>
       </c>
       <c r="D63">
-        <v>1.9020172910662825</v>
+        <v>1.8846373500856652</v>
       </c>
       <c r="E63">
         <v>1</v>
       </c>
       <c r="F63">
-        <v>.49019607843137253</v>
+        <v>.5319148936170213</v>
       </c>
       <c r="G63" t="s">
         <v>23</v>
@@ -2814,7 +3047,7 @@
         <v>-1.4</v>
       </c>
       <c r="I63">
-        <v>-13</v>
+        <v>-12.4</v>
       </c>
       <c r="J63" t="s">
         <v>148</v>
@@ -2822,34 +3055,538 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>149</v>
+        <v>200</v>
       </c>
       <c r="B64" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
       <c r="C64">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D64">
-        <v>24.956772334293948</v>
+        <v>24.785836664762993</v>
       </c>
       <c r="E64">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F64">
-        <v>16.176470588235293</v>
+        <v>17.02127659574468</v>
       </c>
       <c r="G64" t="s">
         <v>23</v>
       </c>
       <c r="H64">
-        <v>-8.8</v>
+        <v>-7.8</v>
       </c>
       <c r="I64">
-        <v>-21.9</v>
+        <v>-19.2</v>
       </c>
       <c r="J64" t="s">
         <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K1048576"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J1" t="s">
+        <v>211</v>
+      </c>
+      <c r="K1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2">
+        <v>2.842371076632776</v>
+      </c>
+      <c r="C2">
+        <v>2.2484597497045615</v>
+      </c>
+      <c r="D2">
+        <v>3.593158978425174</v>
+      </c>
+      <c r="E2">
+        <v>1.0446385899878443</v>
+      </c>
+      <c r="F2">
+        <v>.1195905464194602</v>
+      </c>
+      <c r="G2">
+        <v>.05</v>
+      </c>
+      <c r="H2">
+        <v>.8102454261142368</v>
+      </c>
+      <c r="I2">
+        <v>1.2790317538614517</v>
+      </c>
+      <c r="J2">
+        <v>76.30244064048001</v>
+      </c>
+      <c r="K2">
+        <v>2.4338290640595513e-18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E3">
+        <v>2.842371076632776</v>
+      </c>
+      <c r="F3">
+        <v>.33992071018138303</v>
+      </c>
+      <c r="G3">
+        <v>.05</v>
+      </c>
+      <c r="H3">
+        <v>2.2484597497045615</v>
+      </c>
+      <c r="I3">
+        <v>3.593158978425174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4">
+        <v>1.5805438885033687</v>
+      </c>
+      <c r="C4">
+        <v>1.1566289432824042</v>
+      </c>
+      <c r="D4">
+        <v>2.159827486588674</v>
+      </c>
+      <c r="E4">
+        <v>.4577690210341906</v>
+      </c>
+      <c r="F4">
+        <v>.15931891229396167</v>
+      </c>
+      <c r="G4">
+        <v>.05</v>
+      </c>
+      <c r="H4">
+        <v>.14550969088193005</v>
+      </c>
+      <c r="I4">
+        <v>.7700283511864512</v>
+      </c>
+      <c r="J4">
+        <v>8.255780402139493</v>
+      </c>
+      <c r="K4">
+        <v>.00406224403175378</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E5">
+        <v>1.5805438885033687</v>
+      </c>
+      <c r="F5">
+        <v>.2518105331492253</v>
+      </c>
+      <c r="G5">
+        <v>.05</v>
+      </c>
+      <c r="H5">
+        <v>1.1566289432824042</v>
+      </c>
+      <c r="I5">
+        <v>2.159827486588674</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B6">
+        <v>1.923130691548656</v>
+      </c>
+      <c r="C6">
+        <v>1.4117763356665411</v>
+      </c>
+      <c r="D6">
+        <v>2.6197008430731863</v>
+      </c>
+      <c r="E6">
+        <v>.6539544266211026</v>
+      </c>
+      <c r="F6">
+        <v>.15770988907841652</v>
+      </c>
+      <c r="G6">
+        <v>.05</v>
+      </c>
+      <c r="H6">
+        <v>.3448487240215994</v>
+      </c>
+      <c r="I6">
+        <v>.9630601292206058</v>
+      </c>
+      <c r="J6">
+        <v>17.194007631196406</v>
+      </c>
+      <c r="K6">
+        <v>3.374992733168661e-05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
+      <c r="E7">
+        <v>1.923130691548656</v>
+      </c>
+      <c r="F7">
+        <v>.30329672804743696</v>
+      </c>
+      <c r="G7">
+        <v>.05</v>
+      </c>
+      <c r="H7">
+        <v>1.4117763356665411</v>
+      </c>
+      <c r="I7">
+        <v>2.6197008430731863</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8">
+        <v>1.4135696614382558</v>
+      </c>
+      <c r="C8">
+        <v>.9449951211908217</v>
+      </c>
+      <c r="D8">
+        <v>2.1144862475275947</v>
+      </c>
+      <c r="E8">
+        <v>.34611817987895893</v>
+      </c>
+      <c r="F8">
+        <v>.20545974176980394</v>
+      </c>
+      <c r="G8">
+        <v>.05</v>
+      </c>
+      <c r="H8">
+        <v>-.05657551426275664</v>
+      </c>
+      <c r="I8">
+        <v>.7488118740206745</v>
+      </c>
+      <c r="J8">
+        <v>2.837888620709997</v>
+      </c>
+      <c r="K8">
+        <v>.0920651146357443</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>220</v>
+      </c>
+      <c r="E9">
+        <v>1.4135696614382558</v>
+      </c>
+      <c r="F9">
+        <v>.2904316576127332</v>
+      </c>
+      <c r="G9">
+        <v>.05</v>
+      </c>
+      <c r="H9">
+        <v>.9449951211908217</v>
+      </c>
+      <c r="I9">
+        <v>2.1144862475275947</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B10">
+        <v>1.9167446342539471</v>
+      </c>
+      <c r="C10">
+        <v>1.2907460878399877</v>
+      </c>
+      <c r="D10">
+        <v>2.8463460223144583</v>
+      </c>
+      <c r="E10">
+        <v>.6506282440549817</v>
+      </c>
+      <c r="F10">
+        <v>.20174239594242402</v>
+      </c>
+      <c r="G10">
+        <v>.05</v>
+      </c>
+      <c r="H10">
+        <v>.255220413853011</v>
+      </c>
+      <c r="I10">
+        <v>1.0460360742569523</v>
+      </c>
+      <c r="J10">
+        <v>10.4009132931971</v>
+      </c>
+      <c r="K10">
+        <v>.001259530029184875</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>222</v>
+      </c>
+      <c r="E11">
+        <v>1.9167446342539471</v>
+      </c>
+      <c r="F11">
+        <v>.38668865492417653</v>
+      </c>
+      <c r="G11">
+        <v>.05</v>
+      </c>
+      <c r="H11">
+        <v>1.2907460878399877</v>
+      </c>
+      <c r="I11">
+        <v>2.8463460223144583</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B12">
+        <v>1.5041332429795058</v>
+      </c>
+      <c r="C12">
+        <v>.9133053966683429</v>
+      </c>
+      <c r="D12">
+        <v>2.47717447076207</v>
+      </c>
+      <c r="E12">
+        <v>.40821681401015886</v>
+      </c>
+      <c r="F12">
+        <v>.25454639690870784</v>
+      </c>
+      <c r="G12">
+        <v>.05</v>
+      </c>
+      <c r="H12">
+        <v>-.09068495632534629</v>
+      </c>
+      <c r="I12">
+        <v>.907118584345664</v>
+      </c>
+      <c r="J12">
+        <v>2.571863232176736</v>
+      </c>
+      <c r="K12">
+        <v>.10877953982174415</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>224</v>
+      </c>
+      <c r="E13">
+        <v>1.5041332429795058</v>
+      </c>
+      <c r="F13">
+        <v>.38287169747104316</v>
+      </c>
+      <c r="G13">
+        <v>.05</v>
+      </c>
+      <c r="H13">
+        <v>.9133053966683429</v>
+      </c>
+      <c r="I13">
+        <v>2.47717447076207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>225</v>
+      </c>
+      <c r="B14">
+        <v>1.2790330948877768</v>
+      </c>
+      <c r="C14">
+        <v>.702988508818094</v>
+      </c>
+      <c r="D14">
+        <v>2.327101563251183</v>
+      </c>
+      <c r="E14">
+        <v>.24610439785832344</v>
+      </c>
+      <c r="F14">
+        <v>.30537251490570316</v>
+      </c>
+      <c r="G14">
+        <v>.05</v>
+      </c>
+      <c r="H14">
+        <v>-.35241473322527567</v>
+      </c>
+      <c r="I14">
+        <v>.8446235289419226</v>
+      </c>
+      <c r="J14">
+        <v>.6494995546788473</v>
+      </c>
+      <c r="K14">
+        <v>.4202916586303206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>226</v>
+      </c>
+      <c r="E15">
+        <v>1.2790330948877768</v>
+      </c>
+      <c r="F15">
+        <v>.39058155283350526</v>
+      </c>
+      <c r="G15">
+        <v>.05</v>
+      </c>
+      <c r="H15">
+        <v>.702988508818094</v>
+      </c>
+      <c r="I15">
+        <v>2.327101563251183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>227</v>
+      </c>
+      <c r="B16">
+        <v>1.028373735094613</v>
+      </c>
+      <c r="C16">
+        <v>.7632969514887247</v>
+      </c>
+      <c r="D16">
+        <v>1.3855060431851691</v>
+      </c>
+      <c r="E16">
+        <v>.02797865650217788</v>
+      </c>
+      <c r="F16">
+        <v>.15208789186762303</v>
+      </c>
+      <c r="G16">
+        <v>.05</v>
+      </c>
+      <c r="H16">
+        <v>-.27010813404298545</v>
+      </c>
+      <c r="I16">
+        <v>.32606544704734125</v>
+      </c>
+      <c r="J16">
+        <v>.033842655470820465</v>
+      </c>
+      <c r="K16">
+        <v>.8540419052981808</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>228</v>
+      </c>
+      <c r="E17">
+        <v>1.028373735094613</v>
+      </c>
+      <c r="F17">
+        <v>.1564031934225731</v>
+      </c>
+      <c r="G17">
+        <v>.05</v>
+      </c>
+      <c r="H17">
+        <v>.7632969514887247</v>
+      </c>
+      <c r="I17">
+        <v>1.3855060431851691</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checking the py problem for collapsed sensitivity analysis
</commit_message>
<xml_diff>
--- a/3.output/mnd.xlsx
+++ b/3.output/mnd.xlsx
@@ -8,30 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LabPCSLi03\Desktop\mnd project\3.output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E9B224-6871-451C-9530-91967A594C71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B593D743-0F6D-4804-B5A6-7ECE2A18E6A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="270" windowWidth="11100" windowHeight="5325" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="270" windowWidth="11100" windowHeight="5325" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table 1 demo" sheetId="1" r:id="rId1"/>
-    <sheet name="primary_analysis" sheetId="2" r:id="rId2"/>
-    <sheet name="sub_ae" sheetId="3" r:id="rId3"/>
-    <sheet name="subgroup_pneumonia" sheetId="4" r:id="rId7"/>
-    <sheet name="subgroup_arf" sheetId="5" r:id="rId8"/>
+    <sheet name="primary_analysis1" sheetId="2" r:id="rId2"/>
+    <sheet name="primary_analysis" sheetId="3" r:id="rId3"/>
+    <sheet name="sub_ae" sheetId="4" r:id="rId4"/>
+    <sheet name="subgroup_pneumonia" sheetId="5" r:id="rId5"/>
+    <sheet name="subgroup_arf" sheetId="6" r:id="rId6"/>
+    <sheet name="sensitivity_collapse" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="sub_ae">sub_ae!$A$1:$K$17</definedName>
+    <definedName name="sensitivity_collapse">sensitivity_collapse!$A$1:$G$7</definedName>
+    <definedName name="sub_ae">sub_ae!$A$1:$G$10</definedName>
+    <definedName name="subgroup_arf">subgroup_arf!$A$1:$G$10</definedName>
+    <definedName name="subgroup_pneumonia">subgroup_pneumonia!$A$1:$G$10</definedName>
     <definedName name="table_1_demo">'table 1 demo'!$A$1:$J$64</definedName>
-    <definedName name="primary_analysis">'primary_analysis'!$A$1:$K$17</definedName>
-    <definedName name="subgroup_pneumonia">'subgroup_pneumonia'!$A$1:$K$17</definedName>
-    <definedName name="subgroup_arf">'subgroup_arf'!$A$1:$K$17</definedName>
+    <definedName name="primary_analysis">'primary_analysis'!$A$1:$G$7</definedName>
   </definedNames>
   <calcPr fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
   <si>
     <t>treatment_column</t>
   </si>
@@ -571,6 +574,21 @@
   </si>
   <si>
     <t>Exp(strx_180a)</t>
+  </si>
+  <si>
+    <t>risk_period</t>
+  </si>
+  <si>
+    <t>no_people</t>
+  </si>
+  <si>
+    <t>no_py</t>
+  </si>
+  <si>
+    <t>pvalue</t>
+  </si>
+  <si>
+    <t>baseline</t>
   </si>
 </sst>
 </file>
@@ -2999,514 +3017,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1048576"/>
-  <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J1" t="s">
-        <v>162</v>
-      </c>
-      <c r="K1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B2">
-        <v>2.842371076632773</v>
-      </c>
-      <c r="C2">
-        <v>2.248459749704559</v>
-      </c>
-      <c r="D2">
-        <v>3.593158978425171</v>
-      </c>
-      <c r="E2">
-        <v>1.0446385899878432</v>
-      </c>
-      <c r="F2">
-        <v>.11959054641946029</v>
-      </c>
-      <c r="G2">
-        <v>.05</v>
-      </c>
-      <c r="H2">
-        <v>.8102454261142356</v>
-      </c>
-      <c r="I2">
-        <v>1.2790317538614508</v>
-      </c>
-      <c r="J2">
-        <v>76.30244064047973</v>
-      </c>
-      <c r="K2">
-        <v>2.433829064059847e-18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E3">
-        <v>2.842371076632773</v>
-      </c>
-      <c r="F3">
-        <v>.339920710181383</v>
-      </c>
-      <c r="G3">
-        <v>.05</v>
-      </c>
-      <c r="H3">
-        <v>2.248459749704559</v>
-      </c>
-      <c r="I3">
-        <v>3.593158978425171</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>166</v>
-      </c>
-      <c r="B4">
-        <v>1.5805438885033691</v>
-      </c>
-      <c r="C4">
-        <v>1.1566289432824046</v>
-      </c>
-      <c r="D4">
-        <v>2.1598274865886746</v>
-      </c>
-      <c r="E4">
-        <v>.45776902103419087</v>
-      </c>
-      <c r="F4">
-        <v>.15931891229396164</v>
-      </c>
-      <c r="G4">
-        <v>.05</v>
-      </c>
-      <c r="H4">
-        <v>.1455096908819304</v>
-      </c>
-      <c r="I4">
-        <v>.7700283511864514</v>
-      </c>
-      <c r="J4">
-        <v>8.255780402139507</v>
-      </c>
-      <c r="K4">
-        <v>.004062244031753759</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>167</v>
-      </c>
-      <c r="E5">
-        <v>1.5805438885033691</v>
-      </c>
-      <c r="F5">
-        <v>.25181053314922536</v>
-      </c>
-      <c r="G5">
-        <v>.05</v>
-      </c>
-      <c r="H5">
-        <v>1.1566289432824046</v>
-      </c>
-      <c r="I5">
-        <v>2.1598274865886746</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B6">
-        <v>1.9231306915486532</v>
-      </c>
-      <c r="C6">
-        <v>1.4117763356665396</v>
-      </c>
-      <c r="D6">
-        <v>2.619700843073182</v>
-      </c>
-      <c r="E6">
-        <v>.6539544266211011</v>
-      </c>
-      <c r="F6">
-        <v>.1577098890784164</v>
-      </c>
-      <c r="G6">
-        <v>.05</v>
-      </c>
-      <c r="H6">
-        <v>.34484872402159816</v>
-      </c>
-      <c r="I6">
-        <v>.9630601292206041</v>
-      </c>
-      <c r="J6">
-        <v>17.194007631196357</v>
-      </c>
-      <c r="K6">
-        <v>3.3749927331686936e-05</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E7">
-        <v>1.9231306915486532</v>
-      </c>
-      <c r="F7">
-        <v>.30329672804743635</v>
-      </c>
-      <c r="G7">
-        <v>.05</v>
-      </c>
-      <c r="H7">
-        <v>1.4117763356665396</v>
-      </c>
-      <c r="I7">
-        <v>2.619700843073182</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B8">
-        <v>1.4135696614382565</v>
-      </c>
-      <c r="C8">
-        <v>.9449951211908219</v>
-      </c>
-      <c r="D8">
-        <v>2.1144862475275956</v>
-      </c>
-      <c r="E8">
-        <v>.34611817987895926</v>
-      </c>
-      <c r="F8">
-        <v>.205459741769804</v>
-      </c>
-      <c r="G8">
-        <v>.05</v>
-      </c>
-      <c r="H8">
-        <v>-.05657551426275642</v>
-      </c>
-      <c r="I8">
-        <v>.748811874020675</v>
-      </c>
-      <c r="J8">
-        <v>2.8378886207100016</v>
-      </c>
-      <c r="K8">
-        <v>.09206511463574407</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E9">
-        <v>1.4135696614382565</v>
-      </c>
-      <c r="F9">
-        <v>.29043165761273343</v>
-      </c>
-      <c r="G9">
-        <v>.05</v>
-      </c>
-      <c r="H9">
-        <v>.9449951211908219</v>
-      </c>
-      <c r="I9">
-        <v>2.1144862475275956</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>172</v>
-      </c>
-      <c r="B10">
-        <v>1.9167446342539445</v>
-      </c>
-      <c r="C10">
-        <v>1.2907460878399863</v>
-      </c>
-      <c r="D10">
-        <v>2.846346022314454</v>
-      </c>
-      <c r="E10">
-        <v>.6506282440549802</v>
-      </c>
-      <c r="F10">
-        <v>.2017423959424239</v>
-      </c>
-      <c r="G10">
-        <v>.05</v>
-      </c>
-      <c r="H10">
-        <v>.25522041385300975</v>
-      </c>
-      <c r="I10">
-        <v>1.0460360742569508</v>
-      </c>
-      <c r="J10">
-        <v>10.400913293197064</v>
-      </c>
-      <c r="K10">
-        <v>.001259530029184908</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>173</v>
-      </c>
-      <c r="E11">
-        <v>1.9167446342539445</v>
-      </c>
-      <c r="F11">
-        <v>.38668865492417576</v>
-      </c>
-      <c r="G11">
-        <v>.05</v>
-      </c>
-      <c r="H11">
-        <v>1.2907460878399863</v>
-      </c>
-      <c r="I11">
-        <v>2.846346022314454</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B12">
-        <v>1.504133242979508</v>
-      </c>
-      <c r="C12">
-        <v>.9133053966683445</v>
-      </c>
-      <c r="D12">
-        <v>2.4771744707620735</v>
-      </c>
-      <c r="E12">
-        <v>.4082168140101604</v>
-      </c>
-      <c r="F12">
-        <v>.2545463969087077</v>
-      </c>
-      <c r="G12">
-        <v>.05</v>
-      </c>
-      <c r="H12">
-        <v>-.09068495632534446</v>
-      </c>
-      <c r="I12">
-        <v>.9071185843456653</v>
-      </c>
-      <c r="J12">
-        <v>2.5718632321767587</v>
-      </c>
-      <c r="K12">
-        <v>.10877953982174238</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>175</v>
-      </c>
-      <c r="E13">
-        <v>1.504133242979508</v>
-      </c>
-      <c r="F13">
-        <v>.3828716974710435</v>
-      </c>
-      <c r="G13">
-        <v>.05</v>
-      </c>
-      <c r="H13">
-        <v>.9133053966683445</v>
-      </c>
-      <c r="I13">
-        <v>2.4771744707620735</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>176</v>
-      </c>
-      <c r="B14">
-        <v>1.2790330948877822</v>
-      </c>
-      <c r="C14">
-        <v>.7029885088180978</v>
-      </c>
-      <c r="D14">
-        <v>2.3271015632511904</v>
-      </c>
-      <c r="E14">
-        <v>.2461043978583277</v>
-      </c>
-      <c r="F14">
-        <v>.30537251490570266</v>
-      </c>
-      <c r="G14">
-        <v>.05</v>
-      </c>
-      <c r="H14">
-        <v>-.3524147332252704</v>
-      </c>
-      <c r="I14">
-        <v>.8446235289419258</v>
-      </c>
-      <c r="J14">
-        <v>.6494995546788719</v>
-      </c>
-      <c r="K14">
-        <v>.4202916586303119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>177</v>
-      </c>
-      <c r="E15">
-        <v>1.2790330948877822</v>
-      </c>
-      <c r="F15">
-        <v>.39058155283350626</v>
-      </c>
-      <c r="G15">
-        <v>.05</v>
-      </c>
-      <c r="H15">
-        <v>.7029885088180978</v>
-      </c>
-      <c r="I15">
-        <v>2.3271015632511904</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>178</v>
-      </c>
-      <c r="B16">
-        <v>1.0283737350946125</v>
-      </c>
-      <c r="C16">
-        <v>.7632969514887246</v>
-      </c>
-      <c r="D16">
-        <v>1.3855060431851685</v>
-      </c>
-      <c r="E16">
-        <v>.027978656502177512</v>
-      </c>
-      <c r="F16">
-        <v>.15208789186762298</v>
-      </c>
-      <c r="G16">
-        <v>.05</v>
-      </c>
-      <c r="H16">
-        <v>-.2701081340429857</v>
-      </c>
-      <c r="I16">
-        <v>.32606544704734075</v>
-      </c>
-      <c r="J16">
-        <v>.0338426554708196</v>
-      </c>
-      <c r="K16">
-        <v>.8540419052981827</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>179</v>
-      </c>
-      <c r="E17">
-        <v>1.0283737350946125</v>
-      </c>
-      <c r="F17">
-        <v>.15640319342257297</v>
-      </c>
-      <c r="G17">
-        <v>.05</v>
-      </c>
-      <c r="H17">
-        <v>.7632969514887246</v>
-      </c>
-      <c r="I17">
-        <v>1.3855060431851685</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3556,34 +3070,34 @@
         <v>164</v>
       </c>
       <c r="B2">
-        <v>3.300755013872763</v>
+        <v>2.842371076632773</v>
       </c>
       <c r="C2">
-        <v>2.4432865764449256</v>
+        <v>2.2484597497045589</v>
       </c>
       <c r="D2">
-        <v>4.4591509512808756</v>
+        <v>3.593158978425171</v>
       </c>
       <c r="E2">
-        <v>1.1941512343861729</v>
+        <v>1.0446385899878432</v>
       </c>
       <c r="F2">
-        <v>0.15347585273400827</v>
+        <v>0.11959054641946029</v>
       </c>
       <c r="G2">
         <v>0.05</v>
       </c>
       <c r="H2">
-        <v>0.89334409053094344</v>
+        <v>0.81024542611423556</v>
       </c>
       <c r="I2">
-        <v>1.4949583782414022</v>
+        <v>1.2790317538614508</v>
       </c>
       <c r="J2">
-        <v>60.539461514390801</v>
+        <v>76.30244064047973</v>
       </c>
       <c r="K2">
-        <v>7.2118152410769874E-15</v>
+        <v>2.4338290640598471E-18</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3591,19 +3105,19 @@
         <v>165</v>
       </c>
       <c r="E3">
-        <v>3.300755013872763</v>
+        <v>2.842371076632773</v>
       </c>
       <c r="F3">
-        <v>0.50658619042017561</v>
+        <v>0.33992071018138298</v>
       </c>
       <c r="G3">
         <v>0.05</v>
       </c>
       <c r="H3">
-        <v>2.4432865764449256</v>
+        <v>2.2484597497045589</v>
       </c>
       <c r="I3">
-        <v>4.4591509512808756</v>
+        <v>3.593158978425171</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3611,34 +3125,34 @@
         <v>166</v>
       </c>
       <c r="B4">
-        <v>1.5759422355169879</v>
+        <v>1.5805438885033691</v>
       </c>
       <c r="C4">
-        <v>1.028155905531861</v>
+        <v>1.1566289432824046</v>
       </c>
       <c r="D4">
-        <v>2.415581057623287</v>
+        <v>2.1598274865886746</v>
       </c>
       <c r="E4">
-        <v>0.45485333817322099</v>
+        <v>0.45776902103419087</v>
       </c>
       <c r="F4">
-        <v>0.21790529159231556</v>
+        <v>0.15931891229396164</v>
       </c>
       <c r="G4">
         <v>0.05</v>
       </c>
       <c r="H4">
-        <v>2.7766814611583812E-2</v>
+        <v>0.14550969088193039</v>
       </c>
       <c r="I4">
-        <v>0.88193986173485817</v>
+        <v>0.77002835118645141</v>
       </c>
       <c r="J4">
-        <v>4.3571972335042934</v>
+        <v>8.2557804021395071</v>
       </c>
       <c r="K4">
-        <v>3.6852890386484344E-2</v>
+        <v>4.0622440317537589E-3</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3646,19 +3160,19 @@
         <v>167</v>
       </c>
       <c r="E5">
-        <v>1.5759422355169879</v>
+        <v>1.5805438885033691</v>
       </c>
       <c r="F5">
-        <v>0.34340615236297489</v>
+        <v>0.25181053314922536</v>
       </c>
       <c r="G5">
         <v>0.05</v>
       </c>
       <c r="H5">
-        <v>1.028155905531861</v>
+        <v>1.1566289432824046</v>
       </c>
       <c r="I5">
-        <v>2.415581057623287</v>
+        <v>2.1598274865886746</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3666,34 +3180,34 @@
         <v>168</v>
       </c>
       <c r="B6">
-        <v>2.418731454631827</v>
+        <v>1.9231306915486532</v>
       </c>
       <c r="C6">
-        <v>1.646113666592564</v>
+        <v>1.4117763356665396</v>
       </c>
       <c r="D6">
-        <v>3.5539841314454113</v>
+        <v>2.6197008430731819</v>
       </c>
       <c r="E6">
-        <v>0.88324321043088194</v>
+        <v>0.65395442662110115</v>
       </c>
       <c r="F6">
-        <v>0.19634343148275143</v>
+        <v>0.1577098890784164</v>
       </c>
       <c r="G6">
         <v>0.05</v>
       </c>
       <c r="H6">
-        <v>0.49841715612368132</v>
+        <v>0.34484872402159816</v>
       </c>
       <c r="I6">
-        <v>1.2680692647380827</v>
+        <v>0.96306012922060413</v>
       </c>
       <c r="J6">
-        <v>20.236148678727268</v>
+        <v>17.194007631196357</v>
       </c>
       <c r="K6">
-        <v>6.8447245629175491E-6</v>
+        <v>3.3749927331686936E-5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3701,19 +3215,19 @@
         <v>169</v>
       </c>
       <c r="E7">
-        <v>2.418731454631827</v>
+        <v>1.9231306915486532</v>
       </c>
       <c r="F7">
-        <v>0.47490203363767985</v>
+        <v>0.30329672804743635</v>
       </c>
       <c r="G7">
         <v>0.05</v>
       </c>
       <c r="H7">
-        <v>1.646113666592564</v>
+        <v>1.4117763356665396</v>
       </c>
       <c r="I7">
-        <v>3.5539841314454113</v>
+        <v>2.6197008430731819</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3721,34 +3235,34 @@
         <v>170</v>
       </c>
       <c r="B8">
-        <v>1.6243452227633257</v>
+        <v>1.4135696614382565</v>
       </c>
       <c r="C8">
-        <v>0.96408133429116083</v>
+        <v>0.94499512119082185</v>
       </c>
       <c r="D8">
-        <v>2.7367995923850028</v>
+        <v>2.1144862475275956</v>
       </c>
       <c r="E8">
-        <v>0.48510479474167717</v>
+        <v>0.34611817987895926</v>
       </c>
       <c r="F8">
-        <v>0.26617040676053705</v>
+        <v>0.205459741769804</v>
       </c>
       <c r="G8">
         <v>0.05</v>
       </c>
       <c r="H8">
-        <v>-3.6579616259352077E-2</v>
+        <v>-5.6575514262756421E-2</v>
       </c>
       <c r="I8">
-        <v>1.0067892057427064</v>
+        <v>0.74881187402067495</v>
       </c>
       <c r="J8">
-        <v>3.3216326273589631</v>
+        <v>2.8378886207100016</v>
       </c>
       <c r="K8">
-        <v>6.8373897945768869E-2</v>
+        <v>9.2065114635744072E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3756,19 +3270,19 @@
         <v>171</v>
       </c>
       <c r="E9">
-        <v>1.6243452227633257</v>
+        <v>1.4135696614382565</v>
       </c>
       <c r="F9">
-        <v>0.43235262866244956</v>
+        <v>0.29043165761273343</v>
       </c>
       <c r="G9">
         <v>0.05</v>
       </c>
       <c r="H9">
-        <v>0.96408133429116083</v>
+        <v>0.94499512119082185</v>
       </c>
       <c r="I9">
-        <v>2.7367995923850028</v>
+        <v>2.1144862475275956</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3776,34 +3290,34 @@
         <v>172</v>
       </c>
       <c r="B10">
-        <v>2.432904255551672</v>
+        <v>1.9167446342539445</v>
       </c>
       <c r="C10">
-        <v>1.487440828817983</v>
+        <v>1.2907460878399863</v>
       </c>
       <c r="D10">
-        <v>3.9793334981836375</v>
+        <v>2.8463460223144539</v>
       </c>
       <c r="E10">
-        <v>0.88908571060275599</v>
+        <v>0.65062824405498021</v>
       </c>
       <c r="F10">
-        <v>0.25103962918873213</v>
+        <v>0.20174239594242391</v>
       </c>
       <c r="G10">
         <v>0.05</v>
       </c>
       <c r="H10">
-        <v>0.39705707870055085</v>
+        <v>0.25522041385300975</v>
       </c>
       <c r="I10">
-        <v>1.381114342504961</v>
+        <v>1.0460360742569508</v>
       </c>
       <c r="J10">
-        <v>12.543036646648579</v>
+        <v>10.400913293197064</v>
       </c>
       <c r="K10">
-        <v>3.9768549643681532E-4</v>
+        <v>1.259530029184908E-3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3811,19 +3325,19 @@
         <v>173</v>
       </c>
       <c r="E11">
-        <v>2.432904255551672</v>
+        <v>1.9167446342539445</v>
       </c>
       <c r="F11">
-        <v>0.61075538216538017</v>
+        <v>0.38668865492417576</v>
       </c>
       <c r="G11">
         <v>0.05</v>
       </c>
       <c r="H11">
-        <v>1.487440828817983</v>
+        <v>1.2907460878399863</v>
       </c>
       <c r="I11">
-        <v>3.9793334981836375</v>
+        <v>2.8463460223144539</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3831,34 +3345,34 @@
         <v>174</v>
       </c>
       <c r="B12">
-        <v>2.3565638946721652</v>
+        <v>1.504133242979508</v>
       </c>
       <c r="C12">
-        <v>1.3479881402700011</v>
+        <v>0.91330539666834454</v>
       </c>
       <c r="D12">
-        <v>4.1197642796472254</v>
+        <v>2.4771744707620735</v>
       </c>
       <c r="E12">
-        <v>0.85720458123946874</v>
+        <v>0.40821681401016041</v>
       </c>
       <c r="F12">
-        <v>0.28500083226704204</v>
+        <v>0.25454639690870767</v>
       </c>
       <c r="G12">
         <v>0.05</v>
       </c>
       <c r="H12">
-        <v>0.29861321443212541</v>
+        <v>-9.0684956325344457E-2</v>
       </c>
       <c r="I12">
-        <v>1.4157959480468121</v>
+        <v>0.90711858434566528</v>
       </c>
       <c r="J12">
-        <v>9.0464192371907242</v>
+        <v>2.5718632321767587</v>
       </c>
       <c r="K12">
-        <v>2.632098235074324E-3</v>
+        <v>0.10877953982174238</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3866,19 +3380,19 @@
         <v>175</v>
       </c>
       <c r="E13">
-        <v>2.3565638946721652</v>
+        <v>1.504133242979508</v>
       </c>
       <c r="F13">
-        <v>0.67162267127202913</v>
+        <v>0.38287169747104349</v>
       </c>
       <c r="G13">
         <v>0.05</v>
       </c>
       <c r="H13">
-        <v>1.3479881402700011</v>
+        <v>0.91330539666834454</v>
       </c>
       <c r="I13">
-        <v>4.1197642796472254</v>
+        <v>2.4771744707620735</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3886,34 +3400,34 @@
         <v>176</v>
       </c>
       <c r="B14">
-        <v>1.1716775223628348</v>
+        <v>1.2790330948877822</v>
       </c>
       <c r="C14">
-        <v>0.48313246583835767</v>
+        <v>0.70298850881809782</v>
       </c>
       <c r="D14">
-        <v>2.8415151402175076</v>
+        <v>2.3271015632511904</v>
       </c>
       <c r="E14">
-        <v>0.15843650172613605</v>
+        <v>0.24610439785832769</v>
       </c>
       <c r="F14">
-        <v>0.45199856489755347</v>
+        <v>0.30537251490570266</v>
       </c>
       <c r="G14">
         <v>0.05</v>
       </c>
       <c r="H14">
-        <v>-0.72746440653685918</v>
+        <v>-0.35241473322527039</v>
       </c>
       <c r="I14">
-        <v>1.0443374099891312</v>
+        <v>0.84462352894192583</v>
       </c>
       <c r="J14">
-        <v>0.12286731771644727</v>
+        <v>0.64949955467887188</v>
       </c>
       <c r="K14">
-        <v>0.72594522160518782</v>
+        <v>0.42029165863031193</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3921,19 +3435,19 @@
         <v>177</v>
       </c>
       <c r="E15">
-        <v>1.1716775223628348</v>
+        <v>1.2790330948877822</v>
       </c>
       <c r="F15">
-        <v>0.52959655863072241</v>
+        <v>0.39058155283350626</v>
       </c>
       <c r="G15">
         <v>0.05</v>
       </c>
       <c r="H15">
-        <v>0.48313246583835767</v>
+        <v>0.70298850881809782</v>
       </c>
       <c r="I15">
-        <v>2.8415151402175076</v>
+        <v>2.3271015632511904</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3941,34 +3455,34 @@
         <v>178</v>
       </c>
       <c r="B16">
-        <v>1.2484137122690382</v>
+        <v>1.0283737350946125</v>
       </c>
       <c r="C16">
-        <v>0.83777492271345544</v>
+        <v>0.76329695148872456</v>
       </c>
       <c r="D16">
-        <v>1.8603287765327727</v>
+        <v>1.3855060431851685</v>
       </c>
       <c r="E16">
-        <v>0.22187371522875504</v>
+        <v>2.7978656502177512E-2</v>
       </c>
       <c r="F16">
-        <v>0.2035136980061564</v>
+        <v>0.15208789186762298</v>
       </c>
       <c r="G16">
         <v>0.05</v>
       </c>
       <c r="H16">
-        <v>-0.17700580322387255</v>
+        <v>-0.27010813404298573</v>
       </c>
       <c r="I16">
-        <v>0.62075323368138258</v>
+        <v>0.32606544704734075</v>
       </c>
       <c r="J16">
-        <v>1.1885690564677893</v>
+        <v>3.3842655470819598E-2</v>
       </c>
       <c r="K16">
-        <v>0.27561838466952437</v>
+        <v>0.85404190529818269</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -3976,19 +3490,193 @@
         <v>179</v>
       </c>
       <c r="E17">
-        <v>1.2484137122690382</v>
+        <v>1.0283737350946125</v>
       </c>
       <c r="F17">
-        <v>0.25406929122546568</v>
+        <v>0.15640319342257297</v>
       </c>
       <c r="G17">
         <v>0.05</v>
       </c>
       <c r="H17">
-        <v>0.83777492271345544</v>
+        <v>0.76329695148872456</v>
       </c>
       <c r="I17">
-        <v>1.8603287765327727</v>
+        <v>1.3855060431851685</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1048576"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2">
+        <v>82</v>
+      </c>
+      <c r="C2">
+        <v>80.63244353182752</v>
+      </c>
+      <c r="D2">
+        <v>2.815078796121957</v>
+      </c>
+      <c r="E2">
+        <v>2.227726111310268</v>
+      </c>
+      <c r="F2">
+        <v>3.5572903635422404</v>
+      </c>
+      <c r="G2">
+        <v>4.372304965776837e-18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3">
+        <v>81</v>
+      </c>
+      <c r="C3">
+        <v>131.3620807665982</v>
+      </c>
+      <c r="D3">
+        <v>1.7481906801078708</v>
+      </c>
+      <c r="E3">
+        <v>1.3816668643779235</v>
+      </c>
+      <c r="F3">
+        <v>2.2119446682916717</v>
+      </c>
+      <c r="G3">
+        <v>3.271965590256125e-06</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4">
+        <v>47</v>
+      </c>
+      <c r="C4">
+        <v>89.09240246406571</v>
+      </c>
+      <c r="D4">
+        <v>1.5571495503808483</v>
+      </c>
+      <c r="E4">
+        <v>1.153453900725191</v>
+      </c>
+      <c r="F4">
+        <v>2.102134052108047</v>
+      </c>
+      <c r="G4">
+        <v>.0038236896374536783</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>54.71047227926078</v>
+      </c>
+      <c r="D5">
+        <v>1.3867406493754824</v>
+      </c>
+      <c r="E5">
+        <v>.9338158690357524</v>
+      </c>
+      <c r="F5">
+        <v>2.059345629471957</v>
+      </c>
+      <c r="G5">
+        <v>.10511163231250786</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>112.76112251882273</v>
+      </c>
+      <c r="D6">
+        <v>1.017571259914239</v>
+      </c>
+      <c r="E6">
+        <v>.755521871920583</v>
+      </c>
+      <c r="F6">
+        <v>1.370511308125695</v>
+      </c>
+      <c r="G6">
+        <v>.9087193947595258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7">
+        <v>496</v>
+      </c>
+      <c r="C7">
+        <v>1399.6659822039699</v>
       </c>
     </row>
   </sheetData>
@@ -3998,501 +3686,235 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
-        <v>154</v>
+        <v>181</v>
       </c>
       <c r="C1" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
       <c r="D1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="G1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J1" t="s">
-        <v>162</v>
-      </c>
-      <c r="K1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>164</v>
       </c>
       <c r="B2">
-        <v>1.9965563052859399</v>
+        <v>51</v>
       </c>
       <c r="C2">
-        <v>1.3718759539690293</v>
+        <v>45.149897330595479</v>
       </c>
       <c r="D2">
-        <v>2.9056833226388297</v>
+        <v>3.3007550138727604</v>
       </c>
       <c r="E2">
-        <v>.6914238491199338</v>
+        <v>2.4432865764449234</v>
       </c>
       <c r="F2">
-        <v>.19145491418342445</v>
+        <v>4.4591509512808711</v>
       </c>
       <c r="G2">
-        <v>.05</v>
-      </c>
-      <c r="H2">
-        <v>.3161791126572151</v>
-      </c>
-      <c r="I2">
-        <v>1.0666685855826525</v>
-      </c>
-      <c r="J2">
-        <v>13.042344718526339</v>
-      </c>
-      <c r="K2">
-        <v>.00030452660218670095</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>7.2118152410772398E-15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="B3">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>43.022587268993838</v>
+      </c>
+      <c r="D3">
+        <v>1.5759422355169863</v>
       </c>
       <c r="E3">
-        <v>1.9965563052859399</v>
+        <v>1.0281559055318592</v>
       </c>
       <c r="F3">
-        <v>.3822505160908946</v>
+        <v>2.4155810576232861</v>
       </c>
       <c r="G3">
-        <v>.05</v>
-      </c>
-      <c r="H3">
-        <v>1.3718759539690293</v>
-      </c>
-      <c r="I3">
-        <v>2.9056833226388297</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3.6852890386485038E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B4">
-        <v>1.2737835453270554</v>
+        <v>29</v>
       </c>
       <c r="C4">
-        <v>.7969257046254753</v>
+        <v>35.534565366187543</v>
       </c>
       <c r="D4">
-        <v>2.0359796539735</v>
+        <v>2.4187314546318341</v>
       </c>
       <c r="E4">
-        <v>.24199164108794013</v>
+        <v>1.6461136665925697</v>
       </c>
       <c r="F4">
-        <v>.23928269504588565</v>
+        <v>3.5539841314454188</v>
       </c>
       <c r="G4">
-        <v>.05</v>
-      </c>
-      <c r="H4">
-        <v>-.22699382332567658</v>
-      </c>
-      <c r="I4">
-        <v>.7109771055015568</v>
-      </c>
-      <c r="J4">
-        <v>1.0227703903240062</v>
-      </c>
-      <c r="K4">
-        <v>.31186276495377174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>6.8447245629168986E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>170</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>27.195071868583163</v>
+      </c>
+      <c r="D5">
+        <v>1.6243452227633268</v>
       </c>
       <c r="E5">
-        <v>1.2737835453270554</v>
+        <v>0.96408133429116172</v>
       </c>
       <c r="F5">
-        <v>.30479435963096085</v>
+        <v>2.7367995923850033</v>
       </c>
       <c r="G5">
-        <v>.05</v>
-      </c>
-      <c r="H5">
-        <v>.7969257046254753</v>
-      </c>
-      <c r="I5">
-        <v>2.0359796539735</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>6.8373897945768258E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B6">
-        <v>1.9982117275143203</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>1.330324379283688</v>
+        <v>20.621492128678987</v>
       </c>
       <c r="D6">
-        <v>3.0014109116196988</v>
+        <v>2.4329042555516689</v>
       </c>
       <c r="E6">
-        <v>.6922526443388539</v>
+        <v>1.4874408288179812</v>
       </c>
       <c r="F6">
-        <v>.20757005784458615</v>
+        <v>3.9793334981836348</v>
       </c>
       <c r="G6">
-        <v>.05</v>
-      </c>
-      <c r="H6">
-        <v>.28542280669456926</v>
-      </c>
-      <c r="I6">
-        <v>1.0990824819831386</v>
-      </c>
-      <c r="J6">
-        <v>11.122433916079885</v>
-      </c>
-      <c r="K6">
-        <v>.0008528979198285224</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3.9768549643682399E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>174</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>15.835728952772074</v>
+      </c>
+      <c r="D7">
+        <v>2.3565638946721688</v>
       </c>
       <c r="E7">
-        <v>1.9982117275143203</v>
+        <v>1.3479881402700051</v>
       </c>
       <c r="F7">
-        <v>.4147689238658779</v>
+        <v>4.1197642796472262</v>
       </c>
       <c r="G7">
-        <v>.05</v>
-      </c>
-      <c r="H7">
-        <v>1.330324379283688</v>
-      </c>
-      <c r="I7">
-        <v>3.0014109116196988</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2.632098235074206E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B8">
-        <v>1.2197536248018965</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>.68221853276396</v>
+        <v>12.216290212183436</v>
       </c>
       <c r="D8">
-        <v>2.180824521417872</v>
+        <v>1.1716775223628404</v>
       </c>
       <c r="E8">
-        <v>.19864889146745618</v>
+        <v>0.48313246583836039</v>
       </c>
       <c r="F8">
-        <v>.2964616387052204</v>
+        <v>2.8415151402175196</v>
       </c>
       <c r="G8">
-        <v>.05</v>
-      </c>
-      <c r="H8">
-        <v>-.38240524319250163</v>
-      </c>
-      <c r="I8">
-        <v>.779703026127414</v>
-      </c>
-      <c r="J8">
-        <v>.44898856670941056</v>
-      </c>
-      <c r="K8">
-        <v>.502815659620082</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.7259452216051796</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>178</v>
+      </c>
+      <c r="B9">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>50.803559206023273</v>
+      </c>
+      <c r="D9">
+        <v>1.24841371226904</v>
       </c>
       <c r="E9">
-        <v>1.2197536248018965</v>
+        <v>0.8377749227134571</v>
       </c>
       <c r="F9">
-        <v>.36161015842540284</v>
+        <v>1.8603287765327745</v>
       </c>
       <c r="G9">
-        <v>.05</v>
-      </c>
-      <c r="H9">
-        <v>.68221853276396</v>
-      </c>
-      <c r="I9">
-        <v>2.180824521417872</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.27561838466952082</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="B10">
-        <v>1.8675996960893844</v>
+        <v>258</v>
       </c>
       <c r="C10">
-        <v>1.1058990528857686</v>
-      </c>
-      <c r="D10">
-        <v>3.1539303842711925</v>
-      </c>
-      <c r="E10">
-        <v>.6246540213867372</v>
-      </c>
-      <c r="F10">
-        <v>.2673495017462314</v>
-      </c>
-      <c r="G10">
-        <v>.05</v>
-      </c>
-      <c r="H10">
-        <v>.10065862667939529</v>
-      </c>
-      <c r="I10">
-        <v>1.148649416094079</v>
-      </c>
-      <c r="J10">
-        <v>5.459090855594266</v>
-      </c>
-      <c r="K10">
-        <v>.019466772810687635</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>173</v>
-      </c>
-      <c r="E11">
-        <v>1.8675996960893844</v>
-      </c>
-      <c r="F11">
-        <v>.4993018482109101</v>
-      </c>
-      <c r="G11">
-        <v>.05</v>
-      </c>
-      <c r="H11">
-        <v>1.1058990528857686</v>
-      </c>
-      <c r="I11">
-        <v>3.1539303842711925</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B12">
-        <v>1.2367347054456959</v>
-      </c>
-      <c r="C12">
-        <v>.5822990089453779</v>
-      </c>
-      <c r="D12">
-        <v>2.6266792629855336</v>
-      </c>
-      <c r="E12">
-        <v>.21247460431842255</v>
-      </c>
-      <c r="F12">
-        <v>.3843161468099066</v>
-      </c>
-      <c r="G12">
-        <v>.05</v>
-      </c>
-      <c r="H12">
-        <v>-.5407712021062024</v>
-      </c>
-      <c r="I12">
-        <v>.9657204107430476</v>
-      </c>
-      <c r="J12">
-        <v>.3056587237052661</v>
-      </c>
-      <c r="K12">
-        <v>.5803564651250275</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>175</v>
-      </c>
-      <c r="E13">
-        <v>1.2367347054456959</v>
-      </c>
-      <c r="F13">
-        <v>.47529711662297464</v>
-      </c>
-      <c r="G13">
-        <v>.05</v>
-      </c>
-      <c r="H13">
-        <v>.5822990089453779</v>
-      </c>
-      <c r="I13">
-        <v>2.6266792629855336</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>176</v>
-      </c>
-      <c r="B14">
-        <v>1.4296572999944552</v>
-      </c>
-      <c r="C14">
-        <v>.6728066862871102</v>
-      </c>
-      <c r="D14">
-        <v>3.0379008370247136</v>
-      </c>
-      <c r="E14">
-        <v>.3574347651975534</v>
-      </c>
-      <c r="F14">
-        <v>.3845642080745463</v>
-      </c>
-      <c r="G14">
-        <v>.05</v>
-      </c>
-      <c r="H14">
-        <v>-.3962972323717248</v>
-      </c>
-      <c r="I14">
-        <v>1.1111667627668316</v>
-      </c>
-      <c r="J14">
-        <v>.8638848528987111</v>
-      </c>
-      <c r="K14">
-        <v>.3526538218331019</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>177</v>
-      </c>
-      <c r="E15">
-        <v>1.4296572999944552</v>
-      </c>
-      <c r="F15">
-        <v>.5497950273903617</v>
-      </c>
-      <c r="G15">
-        <v>.05</v>
-      </c>
-      <c r="H15">
-        <v>.6728066862871102</v>
-      </c>
-      <c r="I15">
-        <v>3.0379008370247136</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>178</v>
-      </c>
-      <c r="B16">
-        <v>.8956469469474951</v>
-      </c>
-      <c r="C16">
-        <v>.5902901841903161</v>
-      </c>
-      <c r="D16">
-        <v>1.3589645822701608</v>
-      </c>
-      <c r="E16">
-        <v>-.11020897608305175</v>
-      </c>
-      <c r="F16">
-        <v>.21272434217658834</v>
-      </c>
-      <c r="G16">
-        <v>.05</v>
-      </c>
-      <c r="H16">
-        <v>-.5271410253841398</v>
-      </c>
-      <c r="I16">
-        <v>.30672307321803627</v>
-      </c>
-      <c r="J16">
-        <v>.2684105341754771</v>
-      </c>
-      <c r="K16">
-        <v>.604399997623218</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>179</v>
-      </c>
-      <c r="E17">
-        <v>.8956469469474951</v>
-      </c>
-      <c r="F17">
-        <v>.19052590761187563</v>
-      </c>
-      <c r="G17">
-        <v>.05</v>
-      </c>
-      <c r="H17">
-        <v>.5902901841903161</v>
-      </c>
-      <c r="I17">
-        <v>1.3589645822701608</v>
+        <v>760.29021218343598</v>
       </c>
     </row>
   </sheetData>
@@ -4502,501 +3924,642 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
-        <v>154</v>
+        <v>181</v>
       </c>
       <c r="C1" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
       <c r="D1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="G1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J1" t="s">
-        <v>162</v>
-      </c>
-      <c r="K1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>164</v>
       </c>
       <c r="B2">
-        <v>2.118253518404712</v>
+        <v>31</v>
       </c>
       <c r="C2">
+        <v>41.456536618754278</v>
+      </c>
+      <c r="D2">
+        <v>1.9965563052859399</v>
+      </c>
+      <c r="E2">
+        <v>1.3718759539690293</v>
+      </c>
+      <c r="F2">
+        <v>2.9056833226388297</v>
+      </c>
+      <c r="G2">
+        <v>3.0452660218670095E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>40.854209445585212</v>
+      </c>
+      <c r="D3">
+        <v>1.2737835453270554</v>
+      </c>
+      <c r="E3">
+        <v>0.7969257046254753</v>
+      </c>
+      <c r="F3">
+        <v>2.0359796539735</v>
+      </c>
+      <c r="G3">
+        <v>0.31186276495377174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>36.350444900752912</v>
+      </c>
+      <c r="D4">
+        <v>1.9982117275143203</v>
+      </c>
+      <c r="E4">
+        <v>1.3303243792836881</v>
+      </c>
+      <c r="F4">
+        <v>3.0014109116196988</v>
+      </c>
+      <c r="G4">
+        <v>8.5289791982852241E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>27.816563997262151</v>
+      </c>
+      <c r="D5">
+        <v>1.2197536248018965</v>
+      </c>
+      <c r="E5">
+        <v>0.68221853276396005</v>
+      </c>
+      <c r="F5">
+        <v>2.1808245214178719</v>
+      </c>
+      <c r="G5">
+        <v>0.50281565962008201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>24.238193018480494</v>
+      </c>
+      <c r="D6">
+        <v>1.8675996960893844</v>
+      </c>
+      <c r="E6">
+        <v>1.1058990528857686</v>
+      </c>
+      <c r="F6">
+        <v>3.1539303842711925</v>
+      </c>
+      <c r="G6">
+        <v>1.9466772810687635E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>16.262833675564682</v>
+      </c>
+      <c r="D7">
+        <v>1.2367347054456959</v>
+      </c>
+      <c r="E7">
+        <v>0.58229900894537789</v>
+      </c>
+      <c r="F7">
+        <v>2.6266792629855336</v>
+      </c>
+      <c r="G7">
+        <v>0.58035646512502748</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>14.316221765913758</v>
+      </c>
+      <c r="D8">
+        <v>1.4296572999944552</v>
+      </c>
+      <c r="E8">
+        <v>0.67280668628711016</v>
+      </c>
+      <c r="F8">
+        <v>3.0379008370247136</v>
+      </c>
+      <c r="G8">
+        <v>0.3526538218331019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>58.844626967830251</v>
+      </c>
+      <c r="D9">
+        <v>0.89564694694749514</v>
+      </c>
+      <c r="E9">
+        <v>0.59029018419031609</v>
+      </c>
+      <c r="F9">
+        <v>1.3589645822701608</v>
+      </c>
+      <c r="G9">
+        <v>0.60439999762321805</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10">
+        <v>238</v>
+      </c>
+      <c r="C10">
+        <v>675.1101984941821</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="7" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2">
+        <v>32</v>
+      </c>
+      <c r="C2">
+        <v>41.24572210814511</v>
+      </c>
+      <c r="D2">
+        <v>2.1182535184047122</v>
+      </c>
+      <c r="E2">
         <v>1.4663026478957515</v>
       </c>
+      <c r="F2">
+        <v>3.0600762909847457</v>
+      </c>
+      <c r="G2">
+        <v>6.353082631233649E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>41.634496919917865</v>
+      </c>
+      <c r="D3">
+        <v>1.3895993317984887</v>
+      </c>
+      <c r="E3">
+        <v>0.88093838798384438</v>
+      </c>
+      <c r="F3">
+        <v>2.1919652149046986</v>
+      </c>
+      <c r="G3">
+        <v>0.15711646887589348</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>34.978781656399725</v>
+      </c>
+      <c r="D4">
+        <v>1.8205514118334718</v>
+      </c>
+      <c r="E4">
+        <v>1.1754955283387336</v>
+      </c>
+      <c r="F4">
+        <v>2.8195831997871799</v>
+      </c>
+      <c r="G4">
+        <v>7.2659182987283161E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>25.470225872689937</v>
+      </c>
+      <c r="D5">
+        <v>1.7144905809264182</v>
+      </c>
+      <c r="E5">
+        <v>1.0164889420039505</v>
+      </c>
+      <c r="F5">
+        <v>2.8917953069812956</v>
+      </c>
+      <c r="G5">
+        <v>4.3250683549487745E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>22.072553045858999</v>
+      </c>
+      <c r="D6">
+        <v>1.6976663884805339</v>
+      </c>
+      <c r="E6">
+        <v>0.95050424791727761</v>
+      </c>
+      <c r="F6">
+        <v>3.0321496962182599</v>
+      </c>
+      <c r="G6">
+        <v>7.3706741214279003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>14.376454483230663</v>
+      </c>
+      <c r="D7">
+        <v>1.857629236778968</v>
+      </c>
+      <c r="E7">
+        <v>0.95393914380325084</v>
+      </c>
+      <c r="F7">
+        <v>3.617407256796386</v>
+      </c>
+      <c r="G7">
+        <v>6.8563403882005713E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>12.350444900752908</v>
+      </c>
+      <c r="D8">
+        <v>1.8051768457802204</v>
+      </c>
+      <c r="E8">
+        <v>0.8503902900120035</v>
+      </c>
+      <c r="F8">
+        <v>3.8319621976104976</v>
+      </c>
+      <c r="G8">
+        <v>0.12405233082468414</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>45.34428473648186</v>
+      </c>
+      <c r="D9">
+        <v>1.2775915311715025</v>
+      </c>
+      <c r="E9">
+        <v>0.82363721578698668</v>
+      </c>
+      <c r="F9">
+        <v>1.9817464403445348</v>
+      </c>
+      <c r="G9">
+        <v>0.2740773689803282</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10">
+        <v>258</v>
+      </c>
+      <c r="C10">
+        <v>712.04928131416841</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="7" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2">
+        <v>82</v>
+      </c>
+      <c r="C2">
+        <v>80.632443531827519</v>
+      </c>
       <c r="D2">
-        <v>3.0600762909847457</v>
+        <v>2.815078796121957</v>
       </c>
       <c r="E2">
-        <v>.7505919370910265</v>
+        <v>2.2277261113102682</v>
       </c>
       <c r="F2">
-        <v>.18768095391464956</v>
+        <v>3.5572903635422404</v>
       </c>
       <c r="G2">
-        <v>.05</v>
-      </c>
-      <c r="H2">
-        <v>.3827440268341916</v>
-      </c>
-      <c r="I2">
-        <v>1.1184398473478612</v>
-      </c>
-      <c r="J2">
-        <v>15.994379100005082</v>
-      </c>
-      <c r="K2">
-        <v>6.353082631233649e-05</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4.3723049657768367E-18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="B3">
+        <v>81</v>
+      </c>
+      <c r="C3">
+        <v>131.36208076659821</v>
+      </c>
+      <c r="D3">
+        <v>1.7481906801078708</v>
       </c>
       <c r="E3">
-        <v>2.118253518404712</v>
+        <v>1.3816668643779235</v>
       </c>
       <c r="F3">
-        <v>.3975558409672591</v>
+        <v>2.2119446682916717</v>
       </c>
       <c r="G3">
-        <v>.05</v>
-      </c>
-      <c r="H3">
-        <v>1.4663026478957515</v>
-      </c>
-      <c r="I3">
-        <v>3.0600762909847457</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3.2719655902561251E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B4">
-        <v>1.3895993317984887</v>
+        <v>47</v>
       </c>
       <c r="C4">
-        <v>.8809383879838444</v>
+        <v>89.092402464065714</v>
       </c>
       <c r="D4">
-        <v>2.1919652149046986</v>
+        <v>1.5571495503808483</v>
       </c>
       <c r="E4">
-        <v>.32901545508575414</v>
+        <v>1.1534539007251909</v>
       </c>
       <c r="F4">
-        <v>.2325466428752966</v>
+        <v>2.1021340521080472</v>
       </c>
       <c r="G4">
-        <v>.05</v>
-      </c>
-      <c r="H4">
-        <v>-.1267675896755252</v>
-      </c>
-      <c r="I4">
-        <v>.7847984998470334</v>
-      </c>
-      <c r="J4">
-        <v>2.001762039348837</v>
-      </c>
-      <c r="K4">
-        <v>.15711646887589348</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3.8236896374536783E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>174</v>
+      </c>
+      <c r="B5">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>54.710472279260777</v>
+      </c>
+      <c r="D5">
+        <v>1.3867406493754824</v>
       </c>
       <c r="E5">
-        <v>1.3895993317984887</v>
+        <v>0.93381586903575242</v>
       </c>
       <c r="F5">
-        <v>.32314665955149396</v>
+        <v>2.0593456294719572</v>
       </c>
       <c r="G5">
-        <v>.05</v>
-      </c>
-      <c r="H5">
-        <v>.8809383879838444</v>
-      </c>
-      <c r="I5">
-        <v>2.1919652149046986</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.10511163231250786</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="B6">
-        <v>1.8205514118334718</v>
+        <v>48</v>
       </c>
       <c r="C6">
-        <v>1.1754955283387336</v>
+        <v>112.76112251882273</v>
       </c>
       <c r="D6">
-        <v>2.81958319978718</v>
+        <v>1.017571259914239</v>
       </c>
       <c r="E6">
-        <v>.5991394287363654</v>
+        <v>0.75552187192058295</v>
       </c>
       <c r="F6">
-        <v>.2231926949916318</v>
+        <v>1.370511308125695</v>
       </c>
       <c r="G6">
-        <v>.05</v>
-      </c>
-      <c r="H6">
-        <v>.1616897849403337</v>
-      </c>
-      <c r="I6">
-        <v>1.0365890725323972</v>
-      </c>
-      <c r="J6">
-        <v>7.206026411514321</v>
-      </c>
-      <c r="K6">
-        <v>.007265918298728316</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.90871939475952579</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E7">
-        <v>1.8205514118334718</v>
-      </c>
-      <c r="F7">
-        <v>.40633377597793274</v>
-      </c>
-      <c r="G7">
-        <v>.05</v>
-      </c>
-      <c r="H7">
-        <v>1.1754955283387336</v>
-      </c>
-      <c r="I7">
-        <v>2.81958319978718</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B8">
-        <v>1.7144905809264182</v>
-      </c>
-      <c r="C8">
-        <v>1.0164889420039505</v>
-      </c>
-      <c r="D8">
-        <v>2.8917953069812956</v>
-      </c>
-      <c r="E8">
-        <v>.5391159991328793</v>
-      </c>
-      <c r="F8">
-        <v>.2667199641065086</v>
-      </c>
-      <c r="G8">
-        <v>.05</v>
-      </c>
-      <c r="H8">
-        <v>.016354475526306422</v>
-      </c>
-      <c r="I8">
-        <v>1.0618775227394521</v>
-      </c>
-      <c r="J8">
-        <v>4.085576931943356</v>
-      </c>
-      <c r="K8">
-        <v>.043250683549487745</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E9">
-        <v>1.7144905809264182</v>
-      </c>
-      <c r="F9">
-        <v>.45728886620564135</v>
-      </c>
-      <c r="G9">
-        <v>.05</v>
-      </c>
-      <c r="H9">
-        <v>1.0164889420039505</v>
-      </c>
-      <c r="I9">
-        <v>2.8917953069812956</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>172</v>
-      </c>
-      <c r="B10">
-        <v>1.6976663884805339</v>
-      </c>
-      <c r="C10">
-        <v>.9505042479172776</v>
-      </c>
-      <c r="D10">
-        <v>3.03214969621826</v>
-      </c>
-      <c r="E10">
-        <v>.5292545953705317</v>
-      </c>
-      <c r="F10">
-        <v>.2959326027771842</v>
-      </c>
-      <c r="G10">
-        <v>.05</v>
-      </c>
-      <c r="H10">
-        <v>-.05076264792394736</v>
-      </c>
-      <c r="I10">
-        <v>1.1092718386650107</v>
-      </c>
-      <c r="J10">
-        <v>3.198480058969063</v>
-      </c>
-      <c r="K10">
-        <v>.073706741214279</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>173</v>
-      </c>
-      <c r="E11">
-        <v>1.6976663884805339</v>
-      </c>
-      <c r="F11">
-        <v>.5023948329903867</v>
-      </c>
-      <c r="G11">
-        <v>.05</v>
-      </c>
-      <c r="H11">
-        <v>.9505042479172776</v>
-      </c>
-      <c r="I11">
-        <v>3.03214969621826</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B12">
-        <v>1.857629236778968</v>
-      </c>
-      <c r="C12">
-        <v>.9539391438032508</v>
-      </c>
-      <c r="D12">
-        <v>3.617407256796386</v>
-      </c>
-      <c r="E12">
-        <v>.6193010708443988</v>
-      </c>
-      <c r="F12">
-        <v>.34003505994625793</v>
-      </c>
-      <c r="G12">
-        <v>.05</v>
-      </c>
-      <c r="H12">
-        <v>-.04715540013118513</v>
-      </c>
-      <c r="I12">
-        <v>1.2857575418199827</v>
-      </c>
-      <c r="J12">
-        <v>3.317082443717639</v>
-      </c>
-      <c r="K12">
-        <v>.06856340388200571</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>175</v>
-      </c>
-      <c r="E13">
-        <v>1.857629236778968</v>
-      </c>
-      <c r="F13">
-        <v>.6316590688860577</v>
-      </c>
-      <c r="G13">
-        <v>.05</v>
-      </c>
-      <c r="H13">
-        <v>.9539391438032508</v>
-      </c>
-      <c r="I13">
-        <v>3.617407256796386</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>176</v>
-      </c>
-      <c r="B14">
-        <v>1.8051768457802204</v>
-      </c>
-      <c r="C14">
-        <v>.8503902900120035</v>
-      </c>
-      <c r="D14">
-        <v>3.8319621976104976</v>
-      </c>
-      <c r="E14">
-        <v>.5906585624870654</v>
-      </c>
-      <c r="F14">
-        <v>.3840470736125997</v>
-      </c>
-      <c r="G14">
-        <v>.05</v>
-      </c>
-      <c r="H14">
-        <v>-.16205987016163304</v>
-      </c>
-      <c r="I14">
-        <v>1.3433769951357637</v>
-      </c>
-      <c r="J14">
-        <v>2.365397251329645</v>
-      </c>
-      <c r="K14">
-        <v>.12405233082468414</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>177</v>
-      </c>
-      <c r="E15">
-        <v>1.8051768457802204</v>
-      </c>
-      <c r="F15">
-        <v>.6932728849751169</v>
-      </c>
-      <c r="G15">
-        <v>.05</v>
-      </c>
-      <c r="H15">
-        <v>.8503902900120035</v>
-      </c>
-      <c r="I15">
-        <v>3.8319621976104976</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>178</v>
-      </c>
-      <c r="B16">
-        <v>1.2775915311715025</v>
-      </c>
-      <c r="C16">
-        <v>.8236372157869867</v>
-      </c>
-      <c r="D16">
-        <v>1.9817464403445348</v>
-      </c>
-      <c r="E16">
-        <v>.2449766891956175</v>
-      </c>
-      <c r="F16">
-        <v>.2239846297087415</v>
-      </c>
-      <c r="G16">
-        <v>.05</v>
-      </c>
-      <c r="H16">
-        <v>-.1940251181240561</v>
-      </c>
-      <c r="I16">
-        <v>.6839784965152911</v>
-      </c>
-      <c r="J16">
-        <v>1.1962255868348957</v>
-      </c>
-      <c r="K16">
-        <v>.2740773689803282</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>179</v>
-      </c>
-      <c r="E17">
-        <v>1.2775915311715025</v>
-      </c>
-      <c r="F17">
-        <v>.28616086602847307</v>
-      </c>
-      <c r="G17">
-        <v>.05</v>
-      </c>
-      <c r="H17">
-        <v>.8236372157869867</v>
-      </c>
-      <c r="I17">
-        <v>1.9817464403445348</v>
+        <v>184</v>
+      </c>
+      <c r="B7">
+        <v>496</v>
+      </c>
+      <c r="C7">
+        <v>1399.6659822039699</v>
       </c>
     </row>
   </sheetData>

</xml_diff>